<commit_message>
A lot of codes
</commit_message>
<xml_diff>
--- a/Reference/Civilopedia.xlsx
+++ b/Reference/Civilopedia.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Civilopedia" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="142">
   <si>
     <t>Internal Id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -454,6 +454,14 @@
   </si>
   <si>
     <t>Wonder</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Small Image Asset Path</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Image Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -503,7 +511,13 @@
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -521,26 +535,44 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A1:D120" totalsRowShown="0">
-  <autoFilter ref="A1:D120"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A1:F120" totalsRowShown="0">
+  <autoFilter ref="A1:F120"/>
   <sortState ref="A2:D120">
     <sortCondition ref="B2:B120"/>
     <sortCondition ref="D2:D120"/>
     <sortCondition ref="C2:C120"/>
   </sortState>
-  <tableColumns count="4">
-    <tableColumn id="1" name="Internal Id" dataDxfId="0">
+  <tableColumns count="6">
+    <tableColumn id="1" name="Internal Id" dataDxfId="2">
       <calculatedColumnFormula>CONCATENATE(D2,"-",C2)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" name="Card Type"/>
     <tableColumn id="3" name="Card Name"/>
     <tableColumn id="4" name="Age"/>
+    <tableColumn id="5" name="Small Image Asset Path" dataDxfId="0">
+      <calculatedColumnFormula>_xlfn.CONCAT("SpriteTile/",B2,"s/",LOWER(SUBSTITUTE(C2," ","_")))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" name="Image Name" dataDxfId="1">
+      <calculatedColumnFormula>_xlfn.CONCAT(LOWER(SUBSTITUTE(C2," ","_")))</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A1:A120" totalsRowShown="0">
+  <autoFilter ref="A1:A120"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Output">
+      <calculatedColumnFormula>CONCATENATE(Civilopedia!A2,"|",Civilopedia!B2,"|",Civilopedia!E2)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="B3:B29" totalsRowShown="0">
   <autoFilter ref="B3:B29"/>
   <tableColumns count="1">
@@ -847,10 +879,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D120"/>
+  <dimension ref="A1:F120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -858,9 +890,11 @@
     <col min="1" max="1" width="24.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
     <col min="3" max="3" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -873,10 +907,16 @@
       <c r="D1" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
-        <f>CONCATENATE(D2,"-",C2)</f>
+        <f t="shared" ref="A2:A33" si="0">CONCATENATE(D2,"-",C2)</f>
         <v>0-Cultural Heritage</v>
       </c>
       <c r="B2" t="s">
@@ -888,10 +928,18 @@
       <c r="D2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" t="str">
+        <f t="shared" ref="E2:E33" si="1">_xlfn.CONCAT("SpriteTile/",B2,"s/",LOWER(SUBSTITUTE(C2," ","_")))</f>
+        <v>SpriteTile/Actions/cultural_heritage</v>
+      </c>
+      <c r="F2" t="str">
+        <f t="shared" ref="F2:F33" si="2">_xlfn.CONCAT(LOWER(SUBSTITUTE(C2," ","_")))</f>
+        <v>cultural_heritage</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
-        <f>CONCATENATE(D3,"-",C3)</f>
+        <f t="shared" si="0"/>
         <v>0-Engineering Genius</v>
       </c>
       <c r="B3" t="s">
@@ -903,10 +951,18 @@
       <c r="D3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" t="str">
+        <f t="shared" si="1"/>
+        <v>SpriteTile/Actions/engineering_genius</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" si="2"/>
+        <v>engineering_genius</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
-        <f>CONCATENATE(D4,"-",C4)</f>
+        <f t="shared" si="0"/>
         <v>0-Frugality</v>
       </c>
       <c r="B4" t="s">
@@ -918,10 +974,18 @@
       <c r="D4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" t="str">
+        <f t="shared" si="1"/>
+        <v>SpriteTile/Actions/frugality</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="2"/>
+        <v>frugality</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
-        <f>CONCATENATE(D5,"-",C5)</f>
+        <f t="shared" si="0"/>
         <v>0-Patriotism</v>
       </c>
       <c r="B5" t="s">
@@ -933,10 +997,18 @@
       <c r="D5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" t="str">
+        <f t="shared" si="1"/>
+        <v>SpriteTile/Actions/patriotism</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="2"/>
+        <v>patriotism</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
-        <f>CONCATENATE(D6,"-",C6)</f>
+        <f t="shared" si="0"/>
         <v>0-Rich Land</v>
       </c>
       <c r="B6" t="s">
@@ -948,10 +1020,18 @@
       <c r="D6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" t="str">
+        <f t="shared" si="1"/>
+        <v>SpriteTile/Actions/rich_land</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="2"/>
+        <v>rich_land</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="str">
-        <f>CONCATENATE(D7,"-",C7)</f>
+        <f t="shared" si="0"/>
         <v>0-Stockpile</v>
       </c>
       <c r="B7" t="s">
@@ -963,10 +1043,18 @@
       <c r="D7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7" t="str">
+        <f t="shared" si="1"/>
+        <v>SpriteTile/Actions/stockpile</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="2"/>
+        <v>stockpile</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="str">
-        <f>CONCATENATE(D8,"-",C8)</f>
+        <f t="shared" si="0"/>
         <v>0-Urban Growth</v>
       </c>
       <c r="B8" t="s">
@@ -978,10 +1066,18 @@
       <c r="D8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8" t="str">
+        <f t="shared" si="1"/>
+        <v>SpriteTile/Actions/urban_growth</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="2"/>
+        <v>urban_growth</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="str">
-        <f>CONCATENATE(D9,"-",C9)</f>
+        <f t="shared" si="0"/>
         <v>1-Breakthrough</v>
       </c>
       <c r="B9" t="s">
@@ -993,10 +1089,18 @@
       <c r="D9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9" t="str">
+        <f t="shared" si="1"/>
+        <v>SpriteTile/Actions/breakthrough</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="2"/>
+        <v>breakthrough</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="str">
-        <f>CONCATENATE(D10,"-",C10)</f>
+        <f t="shared" si="0"/>
         <v>1-Cultural Heritage</v>
       </c>
       <c r="B10" t="s">
@@ -1008,10 +1112,18 @@
       <c r="D10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10" t="str">
+        <f t="shared" si="1"/>
+        <v>SpriteTile/Actions/cultural_heritage</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="2"/>
+        <v>cultural_heritage</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="str">
-        <f>CONCATENATE(D11,"-",C11)</f>
+        <f t="shared" si="0"/>
         <v>1-Engineering Genius</v>
       </c>
       <c r="B11" t="s">
@@ -1023,10 +1135,18 @@
       <c r="D11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11" t="str">
+        <f t="shared" si="1"/>
+        <v>SpriteTile/Actions/engineering_genius</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="2"/>
+        <v>engineering_genius</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="str">
-        <f>CONCATENATE(D12,"-",C12)</f>
+        <f t="shared" si="0"/>
         <v>1-Frugality</v>
       </c>
       <c r="B12" t="s">
@@ -1038,10 +1158,18 @@
       <c r="D12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12" t="str">
+        <f t="shared" si="1"/>
+        <v>SpriteTile/Actions/frugality</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="2"/>
+        <v>frugality</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="str">
-        <f>CONCATENATE(D13,"-",C13)</f>
+        <f t="shared" si="0"/>
         <v>1-Patriotism</v>
       </c>
       <c r="B13" t="s">
@@ -1053,10 +1181,18 @@
       <c r="D13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13" t="str">
+        <f t="shared" si="1"/>
+        <v>SpriteTile/Actions/patriotism</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="2"/>
+        <v>patriotism</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="str">
-        <f>CONCATENATE(D14,"-",C14)</f>
+        <f t="shared" si="0"/>
         <v>1-Reserves</v>
       </c>
       <c r="B14" t="s">
@@ -1068,10 +1204,18 @@
       <c r="D14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14" t="str">
+        <f t="shared" si="1"/>
+        <v>SpriteTile/Actions/reserves</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="2"/>
+        <v>reserves</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="str">
-        <f>CONCATENATE(D15,"-",C15)</f>
+        <f t="shared" si="0"/>
         <v>1-Rich Land</v>
       </c>
       <c r="B15" t="s">
@@ -1083,10 +1227,18 @@
       <c r="D15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E15" t="str">
+        <f t="shared" si="1"/>
+        <v>SpriteTile/Actions/rich_land</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="2"/>
+        <v>rich_land</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="str">
-        <f>CONCATENATE(D16,"-",C16)</f>
+        <f t="shared" si="0"/>
         <v>1-Urban Growth</v>
       </c>
       <c r="B16" t="s">
@@ -1098,10 +1250,18 @@
       <c r="D16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16" t="str">
+        <f t="shared" si="1"/>
+        <v>SpriteTile/Actions/urban_growth</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="2"/>
+        <v>urban_growth</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="str">
-        <f>CONCATENATE(D17,"-",C17)</f>
+        <f t="shared" si="0"/>
         <v>2-Breakthrough</v>
       </c>
       <c r="B17" t="s">
@@ -1113,10 +1273,18 @@
       <c r="D17">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17" t="str">
+        <f t="shared" si="1"/>
+        <v>SpriteTile/Actions/breakthrough</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="2"/>
+        <v>breakthrough</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="str">
-        <f>CONCATENATE(D18,"-",C18)</f>
+        <f t="shared" si="0"/>
         <v>2-Efficient Upgrade</v>
       </c>
       <c r="B18" t="s">
@@ -1128,10 +1296,18 @@
       <c r="D18">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18" t="str">
+        <f t="shared" si="1"/>
+        <v>SpriteTile/Actions/efficient_upgrade</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="2"/>
+        <v>efficient_upgrade</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="str">
-        <f>CONCATENATE(D19,"-",C19)</f>
+        <f t="shared" si="0"/>
         <v>2-Engineering Genius</v>
       </c>
       <c r="B19" t="s">
@@ -1143,10 +1319,18 @@
       <c r="D19">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19" t="str">
+        <f t="shared" si="1"/>
+        <v>SpriteTile/Actions/engineering_genius</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="2"/>
+        <v>engineering_genius</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="str">
-        <f>CONCATENATE(D20,"-",C20)</f>
+        <f t="shared" si="0"/>
         <v>2-Frugality</v>
       </c>
       <c r="B20" t="s">
@@ -1158,10 +1342,18 @@
       <c r="D20">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20" t="str">
+        <f t="shared" si="1"/>
+        <v>SpriteTile/Actions/frugality</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="2"/>
+        <v>frugality</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="str">
-        <f>CONCATENATE(D21,"-",C21)</f>
+        <f t="shared" si="0"/>
         <v>2-Patriotism</v>
       </c>
       <c r="B21" t="s">
@@ -1173,10 +1365,18 @@
       <c r="D21">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21" t="str">
+        <f t="shared" si="1"/>
+        <v>SpriteTile/Actions/patriotism</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="2"/>
+        <v>patriotism</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="str">
-        <f>CONCATENATE(D22,"-",C22)</f>
+        <f t="shared" si="0"/>
         <v>2-Reserves</v>
       </c>
       <c r="B22" t="s">
@@ -1188,10 +1388,18 @@
       <c r="D22">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22" t="str">
+        <f t="shared" si="1"/>
+        <v>SpriteTile/Actions/reserves</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" si="2"/>
+        <v>reserves</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="str">
-        <f>CONCATENATE(D23,"-",C23)</f>
+        <f t="shared" si="0"/>
         <v>2-Revolutionary Idea</v>
       </c>
       <c r="B23" t="s">
@@ -1203,10 +1411,18 @@
       <c r="D23">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E23" t="str">
+        <f t="shared" si="1"/>
+        <v>SpriteTile/Actions/revolutionary_idea</v>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" si="2"/>
+        <v>revolutionary_idea</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="str">
-        <f>CONCATENATE(D24,"-",C24)</f>
+        <f t="shared" si="0"/>
         <v>2-Rich Land</v>
       </c>
       <c r="B24" t="s">
@@ -1218,10 +1434,18 @@
       <c r="D24">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E24" t="str">
+        <f t="shared" si="1"/>
+        <v>SpriteTile/Actions/rich_land</v>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" si="2"/>
+        <v>rich_land</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="str">
-        <f>CONCATENATE(D25,"-",C25)</f>
+        <f t="shared" si="0"/>
         <v>2-Urban Growth</v>
       </c>
       <c r="B25" t="s">
@@ -1233,10 +1457,18 @@
       <c r="D25">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E25" t="str">
+        <f t="shared" si="1"/>
+        <v>SpriteTile/Actions/urban_growth</v>
+      </c>
+      <c r="F25" t="str">
+        <f t="shared" si="2"/>
+        <v>urban_growth</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="str">
-        <f>CONCATENATE(D26,"-",C26)</f>
+        <f t="shared" si="0"/>
         <v>2-Wave of Nationalism</v>
       </c>
       <c r="B26" t="s">
@@ -1248,10 +1480,18 @@
       <c r="D26">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E26" t="str">
+        <f t="shared" si="1"/>
+        <v>SpriteTile/Actions/wave_of_nationalism</v>
+      </c>
+      <c r="F26" t="str">
+        <f t="shared" si="2"/>
+        <v>wave_of_nationalism</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="str">
-        <f>CONCATENATE(D27,"-",C27)</f>
+        <f t="shared" si="0"/>
         <v>3-Efficient Upgrade</v>
       </c>
       <c r="B27" t="s">
@@ -1263,10 +1503,18 @@
       <c r="D27">
         <v>3</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E27" t="str">
+        <f t="shared" si="1"/>
+        <v>SpriteTile/Actions/efficient_upgrade</v>
+      </c>
+      <c r="F27" t="str">
+        <f t="shared" si="2"/>
+        <v>efficient_upgrade</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="str">
-        <f>CONCATENATE(D28,"-",C28)</f>
+        <f t="shared" si="0"/>
         <v>3-Endowment for the Arts</v>
       </c>
       <c r="B28" t="s">
@@ -1278,10 +1526,18 @@
       <c r="D28">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E28" t="str">
+        <f t="shared" si="1"/>
+        <v>SpriteTile/Actions/endowment_for_the_arts</v>
+      </c>
+      <c r="F28" t="str">
+        <f t="shared" si="2"/>
+        <v>endowment_for_the_arts</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="str">
-        <f>CONCATENATE(D29,"-",C29)</f>
+        <f t="shared" si="0"/>
         <v>3-Engineering Genius</v>
       </c>
       <c r="B29" t="s">
@@ -1293,10 +1549,18 @@
       <c r="D29">
         <v>3</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E29" t="str">
+        <f t="shared" si="1"/>
+        <v>SpriteTile/Actions/engineering_genius</v>
+      </c>
+      <c r="F29" t="str">
+        <f t="shared" si="2"/>
+        <v>engineering_genius</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="str">
-        <f>CONCATENATE(D30,"-",C30)</f>
+        <f t="shared" si="0"/>
         <v>3-Military Build-Up</v>
       </c>
       <c r="B30" t="s">
@@ -1308,10 +1572,18 @@
       <c r="D30">
         <v>3</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E30" t="str">
+        <f t="shared" si="1"/>
+        <v>SpriteTile/Actions/military_build-up</v>
+      </c>
+      <c r="F30" t="str">
+        <f t="shared" si="2"/>
+        <v>military_build-up</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="str">
-        <f>CONCATENATE(D31,"-",C31)</f>
+        <f t="shared" si="0"/>
         <v>3-Patriotism</v>
       </c>
       <c r="B31" t="s">
@@ -1323,10 +1595,18 @@
       <c r="D31">
         <v>3</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E31" t="str">
+        <f t="shared" si="1"/>
+        <v>SpriteTile/Actions/patriotism</v>
+      </c>
+      <c r="F31" t="str">
+        <f t="shared" si="2"/>
+        <v>patriotism</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="str">
-        <f>CONCATENATE(D32,"-",C32)</f>
+        <f t="shared" si="0"/>
         <v>3-Reserves</v>
       </c>
       <c r="B32" t="s">
@@ -1338,10 +1618,18 @@
       <c r="D32">
         <v>3</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E32" t="str">
+        <f t="shared" si="1"/>
+        <v>SpriteTile/Actions/reserves</v>
+      </c>
+      <c r="F32" t="str">
+        <f t="shared" si="2"/>
+        <v>reserves</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="str">
-        <f>CONCATENATE(D33,"-",C33)</f>
+        <f t="shared" si="0"/>
         <v>3-Revolutionary Idea</v>
       </c>
       <c r="B33" t="s">
@@ -1353,10 +1641,18 @@
       <c r="D33">
         <v>3</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E33" t="str">
+        <f t="shared" si="1"/>
+        <v>SpriteTile/Actions/revolutionary_idea</v>
+      </c>
+      <c r="F33" t="str">
+        <f t="shared" si="2"/>
+        <v>revolutionary_idea</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="str">
-        <f>CONCATENATE(D34,"-",C34)</f>
+        <f t="shared" ref="A34:A65" si="3">CONCATENATE(D34,"-",C34)</f>
         <v>3-Urban Growth</v>
       </c>
       <c r="B34" t="s">
@@ -1368,10 +1664,18 @@
       <c r="D34">
         <v>3</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E34" t="str">
+        <f t="shared" ref="E34:E65" si="4">_xlfn.CONCAT("SpriteTile/",B34,"s/",LOWER(SUBSTITUTE(C34," ","_")))</f>
+        <v>SpriteTile/Actions/urban_growth</v>
+      </c>
+      <c r="F34" t="str">
+        <f t="shared" ref="F34:F65" si="5">_xlfn.CONCAT(LOWER(SUBSTITUTE(C34," ","_")))</f>
+        <v>urban_growth</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="str">
-        <f>CONCATENATE(D35,"-",C35)</f>
+        <f t="shared" si="3"/>
         <v>1-Monarchy</v>
       </c>
       <c r="B35" t="s">
@@ -1383,10 +1687,18 @@
       <c r="D35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E35" t="str">
+        <f t="shared" si="4"/>
+        <v>SpriteTile/Governments/monarchy</v>
+      </c>
+      <c r="F35" t="str">
+        <f t="shared" si="5"/>
+        <v>monarchy</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="str">
-        <f>CONCATENATE(D36,"-",C36)</f>
+        <f t="shared" si="3"/>
         <v>1-Theocracy</v>
       </c>
       <c r="B36" t="s">
@@ -1398,10 +1710,18 @@
       <c r="D36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E36" t="str">
+        <f t="shared" si="4"/>
+        <v>SpriteTile/Governments/theocracy</v>
+      </c>
+      <c r="F36" t="str">
+        <f t="shared" si="5"/>
+        <v>theocracy</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="str">
-        <f>CONCATENATE(D37,"-",C37)</f>
+        <f t="shared" si="3"/>
         <v>2-Constitutional Monarchy</v>
       </c>
       <c r="B37" t="s">
@@ -1413,10 +1733,18 @@
       <c r="D37">
         <v>2</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E37" t="str">
+        <f t="shared" si="4"/>
+        <v>SpriteTile/Governments/constitutional_monarchy</v>
+      </c>
+      <c r="F37" t="str">
+        <f t="shared" si="5"/>
+        <v>constitutional_monarchy</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="str">
-        <f>CONCATENATE(D38,"-",C38)</f>
+        <f t="shared" si="3"/>
         <v>2-Republic</v>
       </c>
       <c r="B38" t="s">
@@ -1428,10 +1756,18 @@
       <c r="D38">
         <v>2</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E38" t="str">
+        <f t="shared" si="4"/>
+        <v>SpriteTile/Governments/republic</v>
+      </c>
+      <c r="F38" t="str">
+        <f t="shared" si="5"/>
+        <v>republic</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="str">
-        <f>CONCATENATE(D39,"-",C39)</f>
+        <f t="shared" si="3"/>
         <v>3-Communism</v>
       </c>
       <c r="B39" t="s">
@@ -1443,10 +1779,18 @@
       <c r="D39">
         <v>3</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E39" t="str">
+        <f t="shared" si="4"/>
+        <v>SpriteTile/Governments/communism</v>
+      </c>
+      <c r="F39" t="str">
+        <f t="shared" si="5"/>
+        <v>communism</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="str">
-        <f>CONCATENATE(D40,"-",C40)</f>
+        <f t="shared" si="3"/>
         <v>3-Democracy</v>
       </c>
       <c r="B40" t="s">
@@ -1458,10 +1802,18 @@
       <c r="D40">
         <v>3</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E40" t="str">
+        <f t="shared" si="4"/>
+        <v>SpriteTile/Governments/democracy</v>
+      </c>
+      <c r="F40" t="str">
+        <f t="shared" si="5"/>
+        <v>democracy</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="str">
-        <f>CONCATENATE(D41,"-",C41)</f>
+        <f t="shared" si="3"/>
         <v>3-Fundamentalism</v>
       </c>
       <c r="B41" t="s">
@@ -1473,10 +1825,18 @@
       <c r="D41">
         <v>3</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E41" t="str">
+        <f t="shared" si="4"/>
+        <v>SpriteTile/Governments/fundamentalism</v>
+      </c>
+      <c r="F41" t="str">
+        <f t="shared" si="5"/>
+        <v>fundamentalism</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="str">
-        <f>CONCATENATE(D42,"-",C42)</f>
+        <f t="shared" si="3"/>
         <v>0-Aristotle</v>
       </c>
       <c r="B42" t="s">
@@ -1488,10 +1848,18 @@
       <c r="D42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E42" t="str">
+        <f t="shared" si="4"/>
+        <v>SpriteTile/Leaders/aristotle</v>
+      </c>
+      <c r="F42" t="str">
+        <f t="shared" si="5"/>
+        <v>aristotle</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="str">
-        <f>CONCATENATE(D43,"-",C43)</f>
+        <f t="shared" si="3"/>
         <v>0-Hammurabi</v>
       </c>
       <c r="B43" t="s">
@@ -1503,10 +1871,18 @@
       <c r="D43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E43" t="str">
+        <f t="shared" si="4"/>
+        <v>SpriteTile/Leaders/hammurabi</v>
+      </c>
+      <c r="F43" t="str">
+        <f t="shared" si="5"/>
+        <v>hammurabi</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="str">
-        <f>CONCATENATE(D44,"-",C44)</f>
+        <f t="shared" si="3"/>
         <v>0-Homer</v>
       </c>
       <c r="B44" t="s">
@@ -1518,10 +1894,18 @@
       <c r="D44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E44" t="str">
+        <f t="shared" si="4"/>
+        <v>SpriteTile/Leaders/homer</v>
+      </c>
+      <c r="F44" t="str">
+        <f t="shared" si="5"/>
+        <v>homer</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="str">
-        <f>CONCATENATE(D45,"-",C45)</f>
+        <f t="shared" si="3"/>
         <v>0-Julius Caesar</v>
       </c>
       <c r="B45" t="s">
@@ -1533,10 +1917,18 @@
       <c r="D45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E45" t="str">
+        <f t="shared" si="4"/>
+        <v>SpriteTile/Leaders/julius_caesar</v>
+      </c>
+      <c r="F45" t="str">
+        <f t="shared" si="5"/>
+        <v>julius_caesar</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="str">
-        <f>CONCATENATE(D46,"-",C46)</f>
+        <f t="shared" si="3"/>
         <v>0-Moses</v>
       </c>
       <c r="B46" t="s">
@@ -1548,10 +1940,18 @@
       <c r="D46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E46" t="str">
+        <f t="shared" si="4"/>
+        <v>SpriteTile/Leaders/moses</v>
+      </c>
+      <c r="F46" t="str">
+        <f t="shared" si="5"/>
+        <v>moses</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="str">
-        <f>CONCATENATE(D47,"-",C47)</f>
+        <f t="shared" si="3"/>
         <v>1-Christopher Columbus</v>
       </c>
       <c r="B47" t="s">
@@ -1563,10 +1963,18 @@
       <c r="D47">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E47" t="str">
+        <f t="shared" si="4"/>
+        <v>SpriteTile/Leaders/christopher_columbus</v>
+      </c>
+      <c r="F47" t="str">
+        <f t="shared" si="5"/>
+        <v>christopher_columbus</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="str">
-        <f>CONCATENATE(D48,"-",C48)</f>
+        <f t="shared" si="3"/>
         <v>1-Genghis Khan</v>
       </c>
       <c r="B48" t="s">
@@ -1578,10 +1986,18 @@
       <c r="D48">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E48" t="str">
+        <f t="shared" si="4"/>
+        <v>SpriteTile/Leaders/genghis_khan</v>
+      </c>
+      <c r="F48" t="str">
+        <f t="shared" si="5"/>
+        <v>genghis_khan</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="str">
-        <f>CONCATENATE(D49,"-",C49)</f>
+        <f t="shared" si="3"/>
         <v>1-Joan of Arc</v>
       </c>
       <c r="B49" t="s">
@@ -1593,10 +2009,18 @@
       <c r="D49">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E49" t="str">
+        <f t="shared" si="4"/>
+        <v>SpriteTile/Leaders/joan_of_arc</v>
+      </c>
+      <c r="F49" t="str">
+        <f t="shared" si="5"/>
+        <v>joan_of_arc</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="str">
-        <f>CONCATENATE(D50,"-",C50)</f>
+        <f t="shared" si="3"/>
         <v>1-Leonardo Da Vinci</v>
       </c>
       <c r="B50" t="s">
@@ -1608,10 +2032,18 @@
       <c r="D50">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E50" t="str">
+        <f t="shared" si="4"/>
+        <v>SpriteTile/Leaders/leonardo_da_vinci</v>
+      </c>
+      <c r="F50" t="str">
+        <f t="shared" si="5"/>
+        <v>leonardo_da_vinci</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="str">
-        <f>CONCATENATE(D51,"-",C51)</f>
+        <f t="shared" si="3"/>
         <v>1-Michelangelo</v>
       </c>
       <c r="B51" t="s">
@@ -1623,10 +2055,18 @@
       <c r="D51">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E51" t="str">
+        <f t="shared" si="4"/>
+        <v>SpriteTile/Leaders/michelangelo</v>
+      </c>
+      <c r="F51" t="str">
+        <f t="shared" si="5"/>
+        <v>michelangelo</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="str">
-        <f>CONCATENATE(D52,"-",C52)</f>
+        <f t="shared" si="3"/>
         <v>2-Frederick Barbarossa</v>
       </c>
       <c r="B52" t="s">
@@ -1638,10 +2078,18 @@
       <c r="D52">
         <v>2</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E52" t="str">
+        <f t="shared" si="4"/>
+        <v>SpriteTile/Leaders/frederick_barbarossa</v>
+      </c>
+      <c r="F52" t="str">
+        <f t="shared" si="5"/>
+        <v>frederick_barbarossa</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="str">
-        <f>CONCATENATE(D53,"-",C53)</f>
+        <f t="shared" si="3"/>
         <v>2-Isaac Newton</v>
       </c>
       <c r="B53" t="s">
@@ -1653,10 +2101,18 @@
       <c r="D53">
         <v>2</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E53" t="str">
+        <f t="shared" si="4"/>
+        <v>SpriteTile/Leaders/isaac_newton</v>
+      </c>
+      <c r="F53" t="str">
+        <f t="shared" si="5"/>
+        <v>isaac_newton</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="str">
-        <f>CONCATENATE(D54,"-",C54)</f>
+        <f t="shared" si="3"/>
         <v>2-James Cook</v>
       </c>
       <c r="B54" t="s">
@@ -1668,10 +2124,18 @@
       <c r="D54">
         <v>2</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E54" t="str">
+        <f t="shared" si="4"/>
+        <v>SpriteTile/Leaders/james_cook</v>
+      </c>
+      <c r="F54" t="str">
+        <f t="shared" si="5"/>
+        <v>james_cook</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="str">
-        <f>CONCATENATE(D55,"-",C55)</f>
+        <f t="shared" si="3"/>
         <v>2-Maximillien Robespierre</v>
       </c>
       <c r="B55" t="s">
@@ -1683,10 +2147,18 @@
       <c r="D55">
         <v>2</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E55" t="str">
+        <f t="shared" si="4"/>
+        <v>SpriteTile/Leaders/maximillien_robespierre</v>
+      </c>
+      <c r="F55" t="str">
+        <f t="shared" si="5"/>
+        <v>maximillien_robespierre</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="str">
-        <f>CONCATENATE(D56,"-",C56)</f>
+        <f t="shared" si="3"/>
         <v>2-Napoleon Bonaparte</v>
       </c>
       <c r="B56" t="s">
@@ -1698,10 +2170,18 @@
       <c r="D56">
         <v>2</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E56" t="str">
+        <f t="shared" si="4"/>
+        <v>SpriteTile/Leaders/napoleon_bonaparte</v>
+      </c>
+      <c r="F56" t="str">
+        <f t="shared" si="5"/>
+        <v>napoleon_bonaparte</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="str">
-        <f>CONCATENATE(D57,"-",C57)</f>
+        <f t="shared" si="3"/>
         <v>2-William Shakespeare</v>
       </c>
       <c r="B57" t="s">
@@ -1713,10 +2193,18 @@
       <c r="D57">
         <v>2</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E57" t="str">
+        <f t="shared" si="4"/>
+        <v>SpriteTile/Leaders/william_shakespeare</v>
+      </c>
+      <c r="F57" t="str">
+        <f t="shared" si="5"/>
+        <v>william_shakespeare</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="str">
-        <f>CONCATENATE(D58,"-",C58)</f>
+        <f t="shared" si="3"/>
         <v>3-Albert Einstein</v>
       </c>
       <c r="B58" t="s">
@@ -1728,10 +2216,18 @@
       <c r="D58">
         <v>3</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E58" t="str">
+        <f t="shared" si="4"/>
+        <v>SpriteTile/Leaders/albert_einstein</v>
+      </c>
+      <c r="F58" t="str">
+        <f t="shared" si="5"/>
+        <v>albert_einstein</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="str">
-        <f>CONCATENATE(D59,"-",C59)</f>
+        <f t="shared" si="3"/>
         <v>3-Bill Gates</v>
       </c>
       <c r="B59" t="s">
@@ -1743,10 +2239,18 @@
       <c r="D59">
         <v>3</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E59" t="str">
+        <f t="shared" si="4"/>
+        <v>SpriteTile/Leaders/bill_gates</v>
+      </c>
+      <c r="F59" t="str">
+        <f t="shared" si="5"/>
+        <v>bill_gates</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="str">
-        <f>CONCATENATE(D60,"-",C60)</f>
+        <f t="shared" si="3"/>
         <v>3-Charles Chaplin</v>
       </c>
       <c r="B60" t="s">
@@ -1758,10 +2262,18 @@
       <c r="D60">
         <v>3</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E60" t="str">
+        <f t="shared" si="4"/>
+        <v>SpriteTile/Leaders/charles_chaplin</v>
+      </c>
+      <c r="F60" t="str">
+        <f t="shared" si="5"/>
+        <v>charles_chaplin</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="str">
-        <f>CONCATENATE(D61,"-",C61)</f>
+        <f t="shared" si="3"/>
         <v>3-Mahatma Gandhi</v>
       </c>
       <c r="B61" t="s">
@@ -1773,10 +2285,18 @@
       <c r="D61">
         <v>3</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E61" t="str">
+        <f t="shared" si="4"/>
+        <v>SpriteTile/Leaders/mahatma_gandhi</v>
+      </c>
+      <c r="F61" t="str">
+        <f t="shared" si="5"/>
+        <v>mahatma_gandhi</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="str">
-        <f>CONCATENATE(D62,"-",C62)</f>
+        <f t="shared" si="3"/>
         <v>3-Sid Meier</v>
       </c>
       <c r="B62" t="s">
@@ -1788,10 +2308,18 @@
       <c r="D62">
         <v>3</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E62" t="str">
+        <f t="shared" si="4"/>
+        <v>SpriteTile/Leaders/sid_meier</v>
+      </c>
+      <c r="F62" t="str">
+        <f t="shared" si="5"/>
+        <v>sid_meier</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="str">
-        <f>CONCATENATE(D63,"-",C63)</f>
+        <f t="shared" si="3"/>
         <v>3-Winston Churchill</v>
       </c>
       <c r="B63" t="s">
@@ -1803,10 +2331,18 @@
       <c r="D63">
         <v>3</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E63" t="str">
+        <f t="shared" si="4"/>
+        <v>SpriteTile/Leaders/winston_churchill</v>
+      </c>
+      <c r="F63" t="str">
+        <f t="shared" si="5"/>
+        <v>winston_churchill</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="str">
-        <f>CONCATENATE(D64,"-",C64)</f>
+        <f t="shared" si="3"/>
         <v>3-Air Forces</v>
       </c>
       <c r="B64" t="s">
@@ -1818,10 +2354,18 @@
       <c r="D64">
         <v>3</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E64" t="str">
+        <f t="shared" si="4"/>
+        <v>SpriteTile/MilitaryTechAirForces/air_forces</v>
+      </c>
+      <c r="F64" t="str">
+        <f t="shared" si="5"/>
+        <v>air_forces</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="str">
-        <f>CONCATENATE(D65,"-",C65)</f>
+        <f t="shared" si="3"/>
         <v>2-Cannon</v>
       </c>
       <c r="B65" t="s">
@@ -1833,10 +2377,18 @@
       <c r="D65">
         <v>2</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E65" t="str">
+        <f t="shared" si="4"/>
+        <v>SpriteTile/MilitaryTechArtillerys/cannon</v>
+      </c>
+      <c r="F65" t="str">
+        <f t="shared" si="5"/>
+        <v>cannon</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="str">
-        <f>CONCATENATE(D66,"-",C66)</f>
+        <f t="shared" ref="A66:A97" si="6">CONCATENATE(D66,"-",C66)</f>
         <v>3-Rockets</v>
       </c>
       <c r="B66" t="s">
@@ -1848,10 +2400,18 @@
       <c r="D66">
         <v>3</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E66" t="str">
+        <f t="shared" ref="E66:E97" si="7">_xlfn.CONCAT("SpriteTile/",B66,"s/",LOWER(SUBSTITUTE(C66," ","_")))</f>
+        <v>SpriteTile/MilitaryTechArtillerys/rockets</v>
+      </c>
+      <c r="F66" t="str">
+        <f t="shared" ref="F66:F97" si="8">_xlfn.CONCAT(LOWER(SUBSTITUTE(C66," ","_")))</f>
+        <v>rockets</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="str">
-        <f>CONCATENATE(D67,"-",C67)</f>
+        <f t="shared" si="6"/>
         <v>1-Knights</v>
       </c>
       <c r="B67" t="s">
@@ -1863,10 +2423,18 @@
       <c r="D67">
         <v>1</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E67" t="str">
+        <f t="shared" si="7"/>
+        <v>SpriteTile/MilitaryTechCavalrys/knights</v>
+      </c>
+      <c r="F67" t="str">
+        <f t="shared" si="8"/>
+        <v>knights</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="str">
-        <f>CONCATENATE(D68,"-",C68)</f>
+        <f t="shared" si="6"/>
         <v>2-Cavalrymen</v>
       </c>
       <c r="B68" t="s">
@@ -1878,10 +2446,18 @@
       <c r="D68">
         <v>2</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E68" t="str">
+        <f t="shared" si="7"/>
+        <v>SpriteTile/MilitaryTechCavalrys/cavalrymen</v>
+      </c>
+      <c r="F68" t="str">
+        <f t="shared" si="8"/>
+        <v>cavalrymen</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="str">
-        <f>CONCATENATE(D69,"-",C69)</f>
+        <f t="shared" si="6"/>
         <v>3-Tanks</v>
       </c>
       <c r="B69" t="s">
@@ -1893,10 +2469,18 @@
       <c r="D69">
         <v>3</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E69" t="str">
+        <f t="shared" si="7"/>
+        <v>SpriteTile/MilitaryTechCavalrys/tanks</v>
+      </c>
+      <c r="F69" t="str">
+        <f t="shared" si="8"/>
+        <v>tanks</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="str">
-        <f>CONCATENATE(D70,"-",C70)</f>
+        <f t="shared" si="6"/>
         <v>1-Swordsmen</v>
       </c>
       <c r="B70" t="s">
@@ -1908,10 +2492,18 @@
       <c r="D70">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E70" t="str">
+        <f t="shared" si="7"/>
+        <v>SpriteTile/MilitaryTechInfantrys/swordsmen</v>
+      </c>
+      <c r="F70" t="str">
+        <f t="shared" si="8"/>
+        <v>swordsmen</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="str">
-        <f>CONCATENATE(D71,"-",C71)</f>
+        <f t="shared" si="6"/>
         <v>2-Riflemen</v>
       </c>
       <c r="B71" t="s">
@@ -1923,10 +2515,18 @@
       <c r="D71">
         <v>2</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E71" t="str">
+        <f t="shared" si="7"/>
+        <v>SpriteTile/MilitaryTechInfantrys/riflemen</v>
+      </c>
+      <c r="F71" t="str">
+        <f t="shared" si="8"/>
+        <v>riflemen</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="str">
-        <f>CONCATENATE(D72,"-",C72)</f>
+        <f t="shared" si="6"/>
         <v>3-Modern Infantry</v>
       </c>
       <c r="B72" t="s">
@@ -1938,10 +2538,18 @@
       <c r="D72">
         <v>3</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E72" t="str">
+        <f t="shared" si="7"/>
+        <v>SpriteTile/MilitaryTechInfantrys/modern_infantry</v>
+      </c>
+      <c r="F72" t="str">
+        <f t="shared" si="8"/>
+        <v>modern_infantry</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="str">
-        <f>CONCATENATE(D73,"-",C73)</f>
+        <f t="shared" si="6"/>
         <v>1-Irrigation</v>
       </c>
       <c r="B73" t="s">
@@ -1953,10 +2561,18 @@
       <c r="D73">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E73" t="str">
+        <f t="shared" si="7"/>
+        <v>SpriteTile/ResourceTechFarms/irrigation</v>
+      </c>
+      <c r="F73" t="str">
+        <f t="shared" si="8"/>
+        <v>irrigation</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" t="str">
-        <f>CONCATENATE(D74,"-",C74)</f>
+        <f t="shared" si="6"/>
         <v>2-Selective Breeding</v>
       </c>
       <c r="B74" t="s">
@@ -1968,10 +2584,18 @@
       <c r="D74">
         <v>2</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E74" t="str">
+        <f t="shared" si="7"/>
+        <v>SpriteTile/ResourceTechFarms/selective_breeding</v>
+      </c>
+      <c r="F74" t="str">
+        <f t="shared" si="8"/>
+        <v>selective_breeding</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="str">
-        <f>CONCATENATE(D75,"-",C75)</f>
+        <f t="shared" si="6"/>
         <v>3-Mechanized Agriculture</v>
       </c>
       <c r="B75" t="s">
@@ -1983,10 +2607,18 @@
       <c r="D75">
         <v>3</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E75" t="str">
+        <f t="shared" si="7"/>
+        <v>SpriteTile/ResourceTechFarms/mechanized_agriculture</v>
+      </c>
+      <c r="F75" t="str">
+        <f t="shared" si="8"/>
+        <v>mechanized_agriculture</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="str">
-        <f>CONCATENATE(D76,"-",C76)</f>
+        <f t="shared" si="6"/>
         <v>1-Iron</v>
       </c>
       <c r="B76" t="s">
@@ -1998,10 +2630,18 @@
       <c r="D76">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E76" t="str">
+        <f t="shared" si="7"/>
+        <v>SpriteTile/ResourceTechMines/iron</v>
+      </c>
+      <c r="F76" t="str">
+        <f t="shared" si="8"/>
+        <v>iron</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="str">
-        <f>CONCATENATE(D77,"-",C77)</f>
+        <f t="shared" si="6"/>
         <v>2-Coal</v>
       </c>
       <c r="B77" t="s">
@@ -2013,10 +2653,18 @@
       <c r="D77">
         <v>2</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E77" t="str">
+        <f t="shared" si="7"/>
+        <v>SpriteTile/ResourceTechMines/coal</v>
+      </c>
+      <c r="F77" t="str">
+        <f t="shared" si="8"/>
+        <v>coal</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="str">
-        <f>CONCATENATE(D78,"-",C78)</f>
+        <f t="shared" si="6"/>
         <v>3-Oil</v>
       </c>
       <c r="B78" t="s">
@@ -2028,10 +2676,18 @@
       <c r="D78">
         <v>3</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E78" t="str">
+        <f t="shared" si="7"/>
+        <v>SpriteTile/ResourceTechMines/oil</v>
+      </c>
+      <c r="F78" t="str">
+        <f t="shared" si="8"/>
+        <v>oil</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" t="str">
-        <f>CONCATENATE(D79,"-",C79)</f>
+        <f t="shared" si="6"/>
         <v>1-Code of Laws</v>
       </c>
       <c r="B79" t="s">
@@ -2043,10 +2699,18 @@
       <c r="D79">
         <v>1</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E79" t="str">
+        <f t="shared" si="7"/>
+        <v>SpriteTile/SpecialTechCivils/code_of_laws</v>
+      </c>
+      <c r="F79" t="str">
+        <f t="shared" si="8"/>
+        <v>code_of_laws</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" t="str">
-        <f>CONCATENATE(D80,"-",C80)</f>
+        <f t="shared" si="6"/>
         <v>2-Justice System</v>
       </c>
       <c r="B80" t="s">
@@ -2058,10 +2722,18 @@
       <c r="D80">
         <v>2</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E80" t="str">
+        <f t="shared" si="7"/>
+        <v>SpriteTile/SpecialTechCivils/justice_system</v>
+      </c>
+      <c r="F80" t="str">
+        <f t="shared" si="8"/>
+        <v>justice_system</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" t="str">
-        <f>CONCATENATE(D81,"-",C81)</f>
+        <f t="shared" si="6"/>
         <v>3-Civil Service</v>
       </c>
       <c r="B81" t="s">
@@ -2073,10 +2745,18 @@
       <c r="D81">
         <v>3</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E81" t="str">
+        <f t="shared" si="7"/>
+        <v>SpriteTile/SpecialTechCivils/civil_service</v>
+      </c>
+      <c r="F81" t="str">
+        <f t="shared" si="8"/>
+        <v>civil_service</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" t="str">
-        <f>CONCATENATE(D82,"-",C82)</f>
+        <f t="shared" si="6"/>
         <v>1-Masonry</v>
       </c>
       <c r="B82" t="s">
@@ -2088,10 +2768,18 @@
       <c r="D82">
         <v>1</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E82" t="str">
+        <f t="shared" si="7"/>
+        <v>SpriteTile/SpecialTechEngineerings/masonry</v>
+      </c>
+      <c r="F82" t="str">
+        <f t="shared" si="8"/>
+        <v>masonry</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" t="str">
-        <f>CONCATENATE(D83,"-",C83)</f>
+        <f t="shared" si="6"/>
         <v>2-Architecture</v>
       </c>
       <c r="B83" t="s">
@@ -2103,10 +2791,18 @@
       <c r="D83">
         <v>2</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E83" t="str">
+        <f t="shared" si="7"/>
+        <v>SpriteTile/SpecialTechEngineerings/architecture</v>
+      </c>
+      <c r="F83" t="str">
+        <f t="shared" si="8"/>
+        <v>architecture</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" t="str">
-        <f>CONCATENATE(D84,"-",C84)</f>
+        <f t="shared" si="6"/>
         <v>3-Engineering</v>
       </c>
       <c r="B84" t="s">
@@ -2118,10 +2814,18 @@
       <c r="D84">
         <v>3</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E84" t="str">
+        <f t="shared" si="7"/>
+        <v>SpriteTile/SpecialTechEngineerings/engineering</v>
+      </c>
+      <c r="F84" t="str">
+        <f t="shared" si="8"/>
+        <v>engineering</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" t="str">
-        <f>CONCATENATE(D85,"-",C85)</f>
+        <f t="shared" si="6"/>
         <v>1-Cartography</v>
       </c>
       <c r="B85" t="s">
@@ -2133,10 +2837,18 @@
       <c r="D85">
         <v>1</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E85" t="str">
+        <f t="shared" si="7"/>
+        <v>SpriteTile/SpecialTechExplorations/cartography</v>
+      </c>
+      <c r="F85" t="str">
+        <f t="shared" si="8"/>
+        <v>cartography</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" t="str">
-        <f>CONCATENATE(D86,"-",C86)</f>
+        <f t="shared" si="6"/>
         <v>2-Navigation</v>
       </c>
       <c r="B86" t="s">
@@ -2148,10 +2860,18 @@
       <c r="D86">
         <v>2</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E86" t="str">
+        <f t="shared" si="7"/>
+        <v>SpriteTile/SpecialTechExplorations/navigation</v>
+      </c>
+      <c r="F86" t="str">
+        <f t="shared" si="8"/>
+        <v>navigation</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" t="str">
-        <f>CONCATENATE(D87,"-",C87)</f>
+        <f t="shared" si="6"/>
         <v>3-Satellites</v>
       </c>
       <c r="B87" t="s">
@@ -2163,10 +2883,18 @@
       <c r="D87">
         <v>3</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E87" t="str">
+        <f t="shared" si="7"/>
+        <v>SpriteTile/SpecialTechExplorations/satellites</v>
+      </c>
+      <c r="F87" t="str">
+        <f t="shared" si="8"/>
+        <v>satellites</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" t="str">
-        <f>CONCATENATE(D88,"-",C88)</f>
+        <f t="shared" si="6"/>
         <v>1-Warfare</v>
       </c>
       <c r="B88" t="s">
@@ -2178,10 +2906,18 @@
       <c r="D88">
         <v>1</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E88" t="str">
+        <f t="shared" si="7"/>
+        <v>SpriteTile/SpecialTechMilitarys/warfare</v>
+      </c>
+      <c r="F88" t="str">
+        <f t="shared" si="8"/>
+        <v>warfare</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" t="str">
-        <f>CONCATENATE(D89,"-",C89)</f>
+        <f t="shared" si="6"/>
         <v>2-Strategy</v>
       </c>
       <c r="B89" t="s">
@@ -2193,10 +2929,18 @@
       <c r="D89">
         <v>2</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E89" t="str">
+        <f t="shared" si="7"/>
+        <v>SpriteTile/SpecialTechMilitarys/strategy</v>
+      </c>
+      <c r="F89" t="str">
+        <f t="shared" si="8"/>
+        <v>strategy</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" t="str">
-        <f>CONCATENATE(D90,"-",C90)</f>
+        <f t="shared" si="6"/>
         <v>3-Military Theory</v>
       </c>
       <c r="B90" t="s">
@@ -2208,10 +2952,18 @@
       <c r="D90">
         <v>3</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E90" t="str">
+        <f t="shared" si="7"/>
+        <v>SpriteTile/SpecialTechMilitarys/military_theory</v>
+      </c>
+      <c r="F90" t="str">
+        <f t="shared" si="8"/>
+        <v>military_theory</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" t="str">
-        <f>CONCATENATE(D91,"-",C91)</f>
+        <f t="shared" si="6"/>
         <v>1-Bread &amp; Circuses</v>
       </c>
       <c r="B91" t="s">
@@ -2223,10 +2975,18 @@
       <c r="D91">
         <v>1</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E91" t="str">
+        <f t="shared" si="7"/>
+        <v>SpriteTile/UrbanTechArenas/bread_&amp;_circuses</v>
+      </c>
+      <c r="F91" t="str">
+        <f t="shared" si="8"/>
+        <v>bread_&amp;_circuses</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" t="str">
-        <f>CONCATENATE(D92,"-",C92)</f>
+        <f t="shared" si="6"/>
         <v>2-Team Sports</v>
       </c>
       <c r="B92" t="s">
@@ -2238,10 +2998,18 @@
       <c r="D92">
         <v>2</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E92" t="str">
+        <f t="shared" si="7"/>
+        <v>SpriteTile/UrbanTechArenas/team_sports</v>
+      </c>
+      <c r="F92" t="str">
+        <f t="shared" si="8"/>
+        <v>team_sports</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" t="str">
-        <f>CONCATENATE(D93,"-",C93)</f>
+        <f t="shared" si="6"/>
         <v>3-Professional Sports</v>
       </c>
       <c r="B93" t="s">
@@ -2253,10 +3021,18 @@
       <c r="D93">
         <v>3</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E93" t="str">
+        <f t="shared" si="7"/>
+        <v>SpriteTile/UrbanTechArenas/professional_sports</v>
+      </c>
+      <c r="F93" t="str">
+        <f t="shared" si="8"/>
+        <v>professional_sports</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" t="str">
-        <f>CONCATENATE(D94,"-",C94)</f>
+        <f t="shared" si="6"/>
         <v>1-Alchemy</v>
       </c>
       <c r="B94" t="s">
@@ -2268,10 +3044,18 @@
       <c r="D94">
         <v>1</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E94" t="str">
+        <f t="shared" si="7"/>
+        <v>SpriteTile/UrbanTechLabs/alchemy</v>
+      </c>
+      <c r="F94" t="str">
+        <f t="shared" si="8"/>
+        <v>alchemy</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" t="str">
-        <f>CONCATENATE(D95,"-",C95)</f>
+        <f t="shared" si="6"/>
         <v>2-Scientific Method</v>
       </c>
       <c r="B95" t="s">
@@ -2283,10 +3067,18 @@
       <c r="D95">
         <v>2</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E95" t="str">
+        <f t="shared" si="7"/>
+        <v>SpriteTile/UrbanTechLabs/scientific_method</v>
+      </c>
+      <c r="F95" t="str">
+        <f t="shared" si="8"/>
+        <v>scientific_method</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" t="str">
-        <f>CONCATENATE(D96,"-",C96)</f>
+        <f t="shared" si="6"/>
         <v>3-Computers</v>
       </c>
       <c r="B96" t="s">
@@ -2298,10 +3090,18 @@
       <c r="D96">
         <v>3</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E96" t="str">
+        <f t="shared" si="7"/>
+        <v>SpriteTile/UrbanTechLabs/computers</v>
+      </c>
+      <c r="F96" t="str">
+        <f t="shared" si="8"/>
+        <v>computers</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" t="str">
-        <f>CONCATENATE(D97,"-",C97)</f>
+        <f t="shared" si="6"/>
         <v>1-Printing Press</v>
       </c>
       <c r="B97" t="s">
@@ -2313,10 +3113,18 @@
       <c r="D97">
         <v>1</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E97" t="str">
+        <f t="shared" si="7"/>
+        <v>SpriteTile/UrbanTechLibrarys/printing_press</v>
+      </c>
+      <c r="F97" t="str">
+        <f t="shared" si="8"/>
+        <v>printing_press</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" t="str">
-        <f>CONCATENATE(D98,"-",C98)</f>
+        <f t="shared" ref="A98:A120" si="9">CONCATENATE(D98,"-",C98)</f>
         <v>2-Journalism</v>
       </c>
       <c r="B98" t="s">
@@ -2328,10 +3136,18 @@
       <c r="D98">
         <v>2</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E98" t="str">
+        <f t="shared" ref="E98:E120" si="10">_xlfn.CONCAT("SpriteTile/",B98,"s/",LOWER(SUBSTITUTE(C98," ","_")))</f>
+        <v>SpriteTile/UrbanTechLibrarys/journalism</v>
+      </c>
+      <c r="F98" t="str">
+        <f t="shared" ref="F98:F120" si="11">_xlfn.CONCAT(LOWER(SUBSTITUTE(C98," ","_")))</f>
+        <v>journalism</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" t="str">
-        <f>CONCATENATE(D99,"-",C99)</f>
+        <f t="shared" si="9"/>
         <v>3-Multimedia</v>
       </c>
       <c r="B99" t="s">
@@ -2343,10 +3159,18 @@
       <c r="D99">
         <v>3</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E99" t="str">
+        <f t="shared" si="10"/>
+        <v>SpriteTile/UrbanTechLibrarys/multimedia</v>
+      </c>
+      <c r="F99" t="str">
+        <f t="shared" si="11"/>
+        <v>multimedia</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" t="str">
-        <f>CONCATENATE(D100,"-",C100)</f>
+        <f t="shared" si="9"/>
         <v>1-Theology</v>
       </c>
       <c r="B100" t="s">
@@ -2358,10 +3182,18 @@
       <c r="D100">
         <v>1</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E100" t="str">
+        <f t="shared" si="10"/>
+        <v>SpriteTile/UrbanTechTemples/theology</v>
+      </c>
+      <c r="F100" t="str">
+        <f t="shared" si="11"/>
+        <v>theology</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" t="str">
-        <f>CONCATENATE(D101,"-",C101)</f>
+        <f t="shared" si="9"/>
         <v>2-Organized Religion</v>
       </c>
       <c r="B101" t="s">
@@ -2373,10 +3205,18 @@
       <c r="D101">
         <v>2</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E101" t="str">
+        <f t="shared" si="10"/>
+        <v>SpriteTile/UrbanTechTemples/organized_religion</v>
+      </c>
+      <c r="F101" t="str">
+        <f t="shared" si="11"/>
+        <v>organized_religion</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" t="str">
-        <f>CONCATENATE(D102,"-",C102)</f>
+        <f t="shared" si="9"/>
         <v>1-Drama</v>
       </c>
       <c r="B102" t="s">
@@ -2388,10 +3228,18 @@
       <c r="D102">
         <v>1</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E102" t="str">
+        <f t="shared" si="10"/>
+        <v>SpriteTile/UrbanTechTheaters/drama</v>
+      </c>
+      <c r="F102" t="str">
+        <f t="shared" si="11"/>
+        <v>drama</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" t="str">
-        <f>CONCATENATE(D103,"-",C103)</f>
+        <f t="shared" si="9"/>
         <v>2-Opera</v>
       </c>
       <c r="B103" t="s">
@@ -2403,10 +3251,18 @@
       <c r="D103">
         <v>2</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E103" t="str">
+        <f t="shared" si="10"/>
+        <v>SpriteTile/UrbanTechTheaters/opera</v>
+      </c>
+      <c r="F103" t="str">
+        <f t="shared" si="11"/>
+        <v>opera</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" t="str">
-        <f>CONCATENATE(D104,"-",C104)</f>
+        <f t="shared" si="9"/>
         <v>3-Movies</v>
       </c>
       <c r="B104" t="s">
@@ -2418,10 +3274,18 @@
       <c r="D104">
         <v>3</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E104" t="str">
+        <f t="shared" si="10"/>
+        <v>SpriteTile/UrbanTechTheaters/movies</v>
+      </c>
+      <c r="F104" t="str">
+        <f t="shared" si="11"/>
+        <v>movies</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" t="str">
-        <f>CONCATENATE(D105,"-",C105)</f>
+        <f t="shared" si="9"/>
         <v>0-Colossus</v>
       </c>
       <c r="B105" t="s">
@@ -2433,10 +3297,18 @@
       <c r="D105">
         <v>0</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E105" t="str">
+        <f t="shared" si="10"/>
+        <v>SpriteTile/Wonders/colossus</v>
+      </c>
+      <c r="F105" t="str">
+        <f t="shared" si="11"/>
+        <v>colossus</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" t="str">
-        <f>CONCATENATE(D106,"-",C106)</f>
+        <f t="shared" si="9"/>
         <v>0-Hanging Gardens</v>
       </c>
       <c r="B106" t="s">
@@ -2448,10 +3320,18 @@
       <c r="D106">
         <v>0</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E106" t="str">
+        <f t="shared" si="10"/>
+        <v>SpriteTile/Wonders/hanging_gardens</v>
+      </c>
+      <c r="F106" t="str">
+        <f t="shared" si="11"/>
+        <v>hanging_gardens</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" t="str">
-        <f>CONCATENATE(D107,"-",C107)</f>
+        <f t="shared" si="9"/>
         <v>0-Library of Alexandria</v>
       </c>
       <c r="B107" t="s">
@@ -2463,10 +3343,18 @@
       <c r="D107">
         <v>0</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E107" t="str">
+        <f t="shared" si="10"/>
+        <v>SpriteTile/Wonders/library_of_alexandria</v>
+      </c>
+      <c r="F107" t="str">
+        <f t="shared" si="11"/>
+        <v>library_of_alexandria</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" t="str">
-        <f>CONCATENATE(D108,"-",C108)</f>
+        <f t="shared" si="9"/>
         <v>0-Pyramids</v>
       </c>
       <c r="B108" t="s">
@@ -2478,10 +3366,18 @@
       <c r="D108">
         <v>0</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E108" t="str">
+        <f t="shared" si="10"/>
+        <v>SpriteTile/Wonders/pyramids</v>
+      </c>
+      <c r="F108" t="str">
+        <f t="shared" si="11"/>
+        <v>pyramids</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" t="str">
-        <f>CONCATENATE(D109,"-",C109)</f>
+        <f t="shared" si="9"/>
         <v>1-Great Wall</v>
       </c>
       <c r="B109" t="s">
@@ -2493,10 +3389,18 @@
       <c r="D109">
         <v>1</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E109" t="str">
+        <f t="shared" si="10"/>
+        <v>SpriteTile/Wonders/great_wall</v>
+      </c>
+      <c r="F109" t="str">
+        <f t="shared" si="11"/>
+        <v>great_wall</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" t="str">
-        <f>CONCATENATE(D110,"-",C110)</f>
+        <f t="shared" si="9"/>
         <v>1-St. Peter's Basilica</v>
       </c>
       <c r="B110" t="s">
@@ -2508,10 +3412,18 @@
       <c r="D110">
         <v>1</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E110" t="str">
+        <f t="shared" si="10"/>
+        <v>SpriteTile/Wonders/st._peter's_basilica</v>
+      </c>
+      <c r="F110" t="str">
+        <f t="shared" si="11"/>
+        <v>st._peter's_basilica</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" t="str">
-        <f>CONCATENATE(D111,"-",C111)</f>
+        <f t="shared" si="9"/>
         <v>1-Taj Mahal</v>
       </c>
       <c r="B111" t="s">
@@ -2523,10 +3435,18 @@
       <c r="D111">
         <v>1</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E111" t="str">
+        <f t="shared" si="10"/>
+        <v>SpriteTile/Wonders/taj_mahal</v>
+      </c>
+      <c r="F111" t="str">
+        <f t="shared" si="11"/>
+        <v>taj_mahal</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" t="str">
-        <f>CONCATENATE(D112,"-",C112)</f>
+        <f t="shared" si="9"/>
         <v>1-Universitas Carolina</v>
       </c>
       <c r="B112" t="s">
@@ -2538,10 +3458,18 @@
       <c r="D112">
         <v>1</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E112" t="str">
+        <f t="shared" si="10"/>
+        <v>SpriteTile/Wonders/universitas_carolina</v>
+      </c>
+      <c r="F112" t="str">
+        <f t="shared" si="11"/>
+        <v>universitas_carolina</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" t="str">
-        <f>CONCATENATE(D113,"-",C113)</f>
+        <f t="shared" si="9"/>
         <v>2-Eiffel Tower</v>
       </c>
       <c r="B113" t="s">
@@ -2553,10 +3481,18 @@
       <c r="D113">
         <v>2</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E113" t="str">
+        <f t="shared" si="10"/>
+        <v>SpriteTile/Wonders/eiffel_tower</v>
+      </c>
+      <c r="F113" t="str">
+        <f t="shared" si="11"/>
+        <v>eiffel_tower</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" t="str">
-        <f>CONCATENATE(D114,"-",C114)</f>
+        <f t="shared" si="9"/>
         <v>2-Kremlin</v>
       </c>
       <c r="B114" t="s">
@@ -2568,10 +3504,18 @@
       <c r="D114">
         <v>2</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E114" t="str">
+        <f t="shared" si="10"/>
+        <v>SpriteTile/Wonders/kremlin</v>
+      </c>
+      <c r="F114" t="str">
+        <f t="shared" si="11"/>
+        <v>kremlin</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" t="str">
-        <f>CONCATENATE(D115,"-",C115)</f>
+        <f t="shared" si="9"/>
         <v>2-Ocean Liner</v>
       </c>
       <c r="B115" t="s">
@@ -2583,10 +3527,18 @@
       <c r="D115">
         <v>2</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E115" t="str">
+        <f t="shared" si="10"/>
+        <v>SpriteTile/Wonders/ocean_liner</v>
+      </c>
+      <c r="F115" t="str">
+        <f t="shared" si="11"/>
+        <v>ocean_liner</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" t="str">
-        <f>CONCATENATE(D116,"-",C116)</f>
+        <f t="shared" si="9"/>
         <v>2-Transcontinental Railroad</v>
       </c>
       <c r="B116" t="s">
@@ -2598,10 +3550,18 @@
       <c r="D116">
         <v>2</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E116" t="str">
+        <f t="shared" si="10"/>
+        <v>SpriteTile/Wonders/transcontinental_railroad</v>
+      </c>
+      <c r="F116" t="str">
+        <f t="shared" si="11"/>
+        <v>transcontinental_railroad</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" t="str">
-        <f>CONCATENATE(D117,"-",C117)</f>
+        <f t="shared" si="9"/>
         <v>3-Fast Food Chains</v>
       </c>
       <c r="B117" t="s">
@@ -2613,10 +3573,18 @@
       <c r="D117">
         <v>3</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E117" t="str">
+        <f t="shared" si="10"/>
+        <v>SpriteTile/Wonders/fast_food_chains</v>
+      </c>
+      <c r="F117" t="str">
+        <f t="shared" si="11"/>
+        <v>fast_food_chains</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" t="str">
-        <f>CONCATENATE(D118,"-",C118)</f>
+        <f t="shared" si="9"/>
         <v>3-First Space Flight</v>
       </c>
       <c r="B118" t="s">
@@ -2628,10 +3596,18 @@
       <c r="D118">
         <v>3</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E118" t="str">
+        <f t="shared" si="10"/>
+        <v>SpriteTile/Wonders/first_space_flight</v>
+      </c>
+      <c r="F118" t="str">
+        <f t="shared" si="11"/>
+        <v>first_space_flight</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" t="str">
-        <f>CONCATENATE(D119,"-",C119)</f>
+        <f t="shared" si="9"/>
         <v>3-Hollywood</v>
       </c>
       <c r="B119" t="s">
@@ -2643,10 +3619,18 @@
       <c r="D119">
         <v>3</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E119" t="str">
+        <f t="shared" si="10"/>
+        <v>SpriteTile/Wonders/hollywood</v>
+      </c>
+      <c r="F119" t="str">
+        <f t="shared" si="11"/>
+        <v>hollywood</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" t="str">
-        <f>CONCATENATE(D120,"-",C120)</f>
+        <f t="shared" si="9"/>
         <v>3-Internet</v>
       </c>
       <c r="B120" t="s">
@@ -2657,6 +3641,14 @@
       </c>
       <c r="D120">
         <v>3</v>
+      </c>
+      <c r="E120" t="str">
+        <f t="shared" si="10"/>
+        <v>SpriteTile/Wonders/internet</v>
+      </c>
+      <c r="F120" t="str">
+        <f t="shared" si="11"/>
+        <v>internet</v>
       </c>
     </row>
   </sheetData>
@@ -2685,8 +3677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A125"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2701,716 +3693,716 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
-        <f>CONCATENATE(Civilopedia!A2,"|",Civilopedia!B2)</f>
-        <v>0-Cultural Heritage|Action</v>
+        <f>CONCATENATE(Civilopedia!A2,"|",Civilopedia!B2,"|",Civilopedia!E2)</f>
+        <v>0-Cultural Heritage|Action|SpriteTile/Actions/cultural_heritage</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
-        <f>CONCATENATE(Civilopedia!A3,"|",Civilopedia!B3)</f>
-        <v>0-Engineering Genius|Action</v>
+        <f>CONCATENATE(Civilopedia!A3,"|",Civilopedia!B3,"|",Civilopedia!E3)</f>
+        <v>0-Engineering Genius|Action|SpriteTile/Actions/engineering_genius</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
-        <f>CONCATENATE(Civilopedia!A4,"|",Civilopedia!B4)</f>
-        <v>0-Frugality|Action</v>
+        <f>CONCATENATE(Civilopedia!A4,"|",Civilopedia!B4,"|",Civilopedia!E4)</f>
+        <v>0-Frugality|Action|SpriteTile/Actions/frugality</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
-        <f>CONCATENATE(Civilopedia!A5,"|",Civilopedia!B5)</f>
-        <v>0-Patriotism|Action</v>
+        <f>CONCATENATE(Civilopedia!A5,"|",Civilopedia!B5,"|",Civilopedia!E5)</f>
+        <v>0-Patriotism|Action|SpriteTile/Actions/patriotism</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
-        <f>CONCATENATE(Civilopedia!A6,"|",Civilopedia!B6)</f>
-        <v>0-Rich Land|Action</v>
+        <f>CONCATENATE(Civilopedia!A6,"|",Civilopedia!B6,"|",Civilopedia!E6)</f>
+        <v>0-Rich Land|Action|SpriteTile/Actions/rich_land</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="str">
-        <f>CONCATENATE(Civilopedia!A7,"|",Civilopedia!B7)</f>
-        <v>0-Stockpile|Action</v>
+        <f>CONCATENATE(Civilopedia!A7,"|",Civilopedia!B7,"|",Civilopedia!E7)</f>
+        <v>0-Stockpile|Action|SpriteTile/Actions/stockpile</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="str">
-        <f>CONCATENATE(Civilopedia!A8,"|",Civilopedia!B8)</f>
-        <v>0-Urban Growth|Action</v>
+        <f>CONCATENATE(Civilopedia!A8,"|",Civilopedia!B8,"|",Civilopedia!E8)</f>
+        <v>0-Urban Growth|Action|SpriteTile/Actions/urban_growth</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="str">
-        <f>CONCATENATE(Civilopedia!A9,"|",Civilopedia!B9)</f>
-        <v>1-Breakthrough|Action</v>
+        <f>CONCATENATE(Civilopedia!A9,"|",Civilopedia!B9,"|",Civilopedia!E9)</f>
+        <v>1-Breakthrough|Action|SpriteTile/Actions/breakthrough</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="str">
-        <f>CONCATENATE(Civilopedia!A10,"|",Civilopedia!B10)</f>
-        <v>1-Cultural Heritage|Action</v>
+        <f>CONCATENATE(Civilopedia!A10,"|",Civilopedia!B10,"|",Civilopedia!E10)</f>
+        <v>1-Cultural Heritage|Action|SpriteTile/Actions/cultural_heritage</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="str">
-        <f>CONCATENATE(Civilopedia!A11,"|",Civilopedia!B11)</f>
-        <v>1-Engineering Genius|Action</v>
+        <f>CONCATENATE(Civilopedia!A11,"|",Civilopedia!B11,"|",Civilopedia!E11)</f>
+        <v>1-Engineering Genius|Action|SpriteTile/Actions/engineering_genius</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="str">
-        <f>CONCATENATE(Civilopedia!A12,"|",Civilopedia!B12)</f>
-        <v>1-Frugality|Action</v>
+        <f>CONCATENATE(Civilopedia!A12,"|",Civilopedia!B12,"|",Civilopedia!E12)</f>
+        <v>1-Frugality|Action|SpriteTile/Actions/frugality</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="str">
-        <f>CONCATENATE(Civilopedia!A13,"|",Civilopedia!B13)</f>
-        <v>1-Patriotism|Action</v>
+        <f>CONCATENATE(Civilopedia!A13,"|",Civilopedia!B13,"|",Civilopedia!E13)</f>
+        <v>1-Patriotism|Action|SpriteTile/Actions/patriotism</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="str">
-        <f>CONCATENATE(Civilopedia!A14,"|",Civilopedia!B14)</f>
-        <v>1-Reserves|Action</v>
+        <f>CONCATENATE(Civilopedia!A14,"|",Civilopedia!B14,"|",Civilopedia!E14)</f>
+        <v>1-Reserves|Action|SpriteTile/Actions/reserves</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="str">
-        <f>CONCATENATE(Civilopedia!A15,"|",Civilopedia!B15)</f>
-        <v>1-Rich Land|Action</v>
+        <f>CONCATENATE(Civilopedia!A15,"|",Civilopedia!B15,"|",Civilopedia!E15)</f>
+        <v>1-Rich Land|Action|SpriteTile/Actions/rich_land</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="str">
-        <f>CONCATENATE(Civilopedia!A16,"|",Civilopedia!B16)</f>
-        <v>1-Urban Growth|Action</v>
+        <f>CONCATENATE(Civilopedia!A16,"|",Civilopedia!B16,"|",Civilopedia!E16)</f>
+        <v>1-Urban Growth|Action|SpriteTile/Actions/urban_growth</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="str">
-        <f>CONCATENATE(Civilopedia!A17,"|",Civilopedia!B17)</f>
-        <v>2-Breakthrough|Action</v>
+        <f>CONCATENATE(Civilopedia!A17,"|",Civilopedia!B17,"|",Civilopedia!E17)</f>
+        <v>2-Breakthrough|Action|SpriteTile/Actions/breakthrough</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="str">
-        <f>CONCATENATE(Civilopedia!A18,"|",Civilopedia!B18)</f>
-        <v>2-Efficient Upgrade|Action</v>
+        <f>CONCATENATE(Civilopedia!A18,"|",Civilopedia!B18,"|",Civilopedia!E18)</f>
+        <v>2-Efficient Upgrade|Action|SpriteTile/Actions/efficient_upgrade</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="str">
-        <f>CONCATENATE(Civilopedia!A19,"|",Civilopedia!B19)</f>
-        <v>2-Engineering Genius|Action</v>
+        <f>CONCATENATE(Civilopedia!A19,"|",Civilopedia!B19,"|",Civilopedia!E19)</f>
+        <v>2-Engineering Genius|Action|SpriteTile/Actions/engineering_genius</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="str">
-        <f>CONCATENATE(Civilopedia!A20,"|",Civilopedia!B20)</f>
-        <v>2-Frugality|Action</v>
+        <f>CONCATENATE(Civilopedia!A20,"|",Civilopedia!B20,"|",Civilopedia!E20)</f>
+        <v>2-Frugality|Action|SpriteTile/Actions/frugality</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="str">
-        <f>CONCATENATE(Civilopedia!A21,"|",Civilopedia!B21)</f>
-        <v>2-Patriotism|Action</v>
+        <f>CONCATENATE(Civilopedia!A21,"|",Civilopedia!B21,"|",Civilopedia!E21)</f>
+        <v>2-Patriotism|Action|SpriteTile/Actions/patriotism</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="str">
-        <f>CONCATENATE(Civilopedia!A22,"|",Civilopedia!B22)</f>
-        <v>2-Reserves|Action</v>
+        <f>CONCATENATE(Civilopedia!A22,"|",Civilopedia!B22,"|",Civilopedia!E22)</f>
+        <v>2-Reserves|Action|SpriteTile/Actions/reserves</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="str">
-        <f>CONCATENATE(Civilopedia!A23,"|",Civilopedia!B23)</f>
-        <v>2-Revolutionary Idea|Action</v>
+        <f>CONCATENATE(Civilopedia!A23,"|",Civilopedia!B23,"|",Civilopedia!E23)</f>
+        <v>2-Revolutionary Idea|Action|SpriteTile/Actions/revolutionary_idea</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="str">
-        <f>CONCATENATE(Civilopedia!A24,"|",Civilopedia!B24)</f>
-        <v>2-Rich Land|Action</v>
+        <f>CONCATENATE(Civilopedia!A24,"|",Civilopedia!B24,"|",Civilopedia!E24)</f>
+        <v>2-Rich Land|Action|SpriteTile/Actions/rich_land</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="str">
-        <f>CONCATENATE(Civilopedia!A25,"|",Civilopedia!B25)</f>
-        <v>2-Urban Growth|Action</v>
+        <f>CONCATENATE(Civilopedia!A25,"|",Civilopedia!B25,"|",Civilopedia!E25)</f>
+        <v>2-Urban Growth|Action|SpriteTile/Actions/urban_growth</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="str">
-        <f>CONCATENATE(Civilopedia!A26,"|",Civilopedia!B26)</f>
-        <v>2-Wave of Nationalism|Action</v>
+        <f>CONCATENATE(Civilopedia!A26,"|",Civilopedia!B26,"|",Civilopedia!E26)</f>
+        <v>2-Wave of Nationalism|Action|SpriteTile/Actions/wave_of_nationalism</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="str">
-        <f>CONCATENATE(Civilopedia!A27,"|",Civilopedia!B27)</f>
-        <v>3-Efficient Upgrade|Action</v>
+        <f>CONCATENATE(Civilopedia!A27,"|",Civilopedia!B27,"|",Civilopedia!E27)</f>
+        <v>3-Efficient Upgrade|Action|SpriteTile/Actions/efficient_upgrade</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="str">
-        <f>CONCATENATE(Civilopedia!A28,"|",Civilopedia!B28)</f>
-        <v>3-Endowment for the Arts|Action</v>
+        <f>CONCATENATE(Civilopedia!A28,"|",Civilopedia!B28,"|",Civilopedia!E28)</f>
+        <v>3-Endowment for the Arts|Action|SpriteTile/Actions/endowment_for_the_arts</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="str">
-        <f>CONCATENATE(Civilopedia!A29,"|",Civilopedia!B29)</f>
-        <v>3-Engineering Genius|Action</v>
+        <f>CONCATENATE(Civilopedia!A29,"|",Civilopedia!B29,"|",Civilopedia!E29)</f>
+        <v>3-Engineering Genius|Action|SpriteTile/Actions/engineering_genius</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="str">
-        <f>CONCATENATE(Civilopedia!A30,"|",Civilopedia!B30)</f>
-        <v>3-Military Build-Up|Action</v>
+        <f>CONCATENATE(Civilopedia!A30,"|",Civilopedia!B30,"|",Civilopedia!E30)</f>
+        <v>3-Military Build-Up|Action|SpriteTile/Actions/military_build-up</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="str">
-        <f>CONCATENATE(Civilopedia!A31,"|",Civilopedia!B31)</f>
-        <v>3-Patriotism|Action</v>
+        <f>CONCATENATE(Civilopedia!A31,"|",Civilopedia!B31,"|",Civilopedia!E31)</f>
+        <v>3-Patriotism|Action|SpriteTile/Actions/patriotism</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="str">
-        <f>CONCATENATE(Civilopedia!A32,"|",Civilopedia!B32)</f>
-        <v>3-Reserves|Action</v>
+        <f>CONCATENATE(Civilopedia!A32,"|",Civilopedia!B32,"|",Civilopedia!E32)</f>
+        <v>3-Reserves|Action|SpriteTile/Actions/reserves</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="str">
-        <f>CONCATENATE(Civilopedia!A33,"|",Civilopedia!B33)</f>
-        <v>3-Revolutionary Idea|Action</v>
+        <f>CONCATENATE(Civilopedia!A33,"|",Civilopedia!B33,"|",Civilopedia!E33)</f>
+        <v>3-Revolutionary Idea|Action|SpriteTile/Actions/revolutionary_idea</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="str">
-        <f>CONCATENATE(Civilopedia!A34,"|",Civilopedia!B34)</f>
-        <v>3-Urban Growth|Action</v>
+        <f>CONCATENATE(Civilopedia!A34,"|",Civilopedia!B34,"|",Civilopedia!E34)</f>
+        <v>3-Urban Growth|Action|SpriteTile/Actions/urban_growth</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="str">
-        <f>CONCATENATE(Civilopedia!A35,"|",Civilopedia!B35)</f>
-        <v>1-Monarchy|Government</v>
+        <f>CONCATENATE(Civilopedia!A35,"|",Civilopedia!B35,"|",Civilopedia!E35)</f>
+        <v>1-Monarchy|Government|SpriteTile/Governments/monarchy</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="str">
-        <f>CONCATENATE(Civilopedia!A36,"|",Civilopedia!B36)</f>
-        <v>1-Theocracy|Government</v>
+        <f>CONCATENATE(Civilopedia!A36,"|",Civilopedia!B36,"|",Civilopedia!E36)</f>
+        <v>1-Theocracy|Government|SpriteTile/Governments/theocracy</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="str">
-        <f>CONCATENATE(Civilopedia!A37,"|",Civilopedia!B37)</f>
-        <v>2-Constitutional Monarchy|Government</v>
+        <f>CONCATENATE(Civilopedia!A37,"|",Civilopedia!B37,"|",Civilopedia!E37)</f>
+        <v>2-Constitutional Monarchy|Government|SpriteTile/Governments/constitutional_monarchy</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="str">
-        <f>CONCATENATE(Civilopedia!A38,"|",Civilopedia!B38)</f>
-        <v>2-Republic|Government</v>
+        <f>CONCATENATE(Civilopedia!A38,"|",Civilopedia!B38,"|",Civilopedia!E38)</f>
+        <v>2-Republic|Government|SpriteTile/Governments/republic</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="str">
-        <f>CONCATENATE(Civilopedia!A39,"|",Civilopedia!B39)</f>
-        <v>3-Communism|Government</v>
+        <f>CONCATENATE(Civilopedia!A39,"|",Civilopedia!B39,"|",Civilopedia!E39)</f>
+        <v>3-Communism|Government|SpriteTile/Governments/communism</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="str">
-        <f>CONCATENATE(Civilopedia!A40,"|",Civilopedia!B40)</f>
-        <v>3-Democracy|Government</v>
+        <f>CONCATENATE(Civilopedia!A40,"|",Civilopedia!B40,"|",Civilopedia!E40)</f>
+        <v>3-Democracy|Government|SpriteTile/Governments/democracy</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="str">
-        <f>CONCATENATE(Civilopedia!A41,"|",Civilopedia!B41)</f>
-        <v>3-Fundamentalism|Government</v>
+        <f>CONCATENATE(Civilopedia!A41,"|",Civilopedia!B41,"|",Civilopedia!E41)</f>
+        <v>3-Fundamentalism|Government|SpriteTile/Governments/fundamentalism</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="str">
-        <f>CONCATENATE(Civilopedia!A42,"|",Civilopedia!B42)</f>
-        <v>0-Aristotle|Leader</v>
+        <f>CONCATENATE(Civilopedia!A42,"|",Civilopedia!B42,"|",Civilopedia!E42)</f>
+        <v>0-Aristotle|Leader|SpriteTile/Leaders/aristotle</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="str">
-        <f>CONCATENATE(Civilopedia!A43,"|",Civilopedia!B43)</f>
-        <v>0-Hammurabi|Leader</v>
+        <f>CONCATENATE(Civilopedia!A43,"|",Civilopedia!B43,"|",Civilopedia!E43)</f>
+        <v>0-Hammurabi|Leader|SpriteTile/Leaders/hammurabi</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="str">
-        <f>CONCATENATE(Civilopedia!A44,"|",Civilopedia!B44)</f>
-        <v>0-Homer|Leader</v>
+        <f>CONCATENATE(Civilopedia!A44,"|",Civilopedia!B44,"|",Civilopedia!E44)</f>
+        <v>0-Homer|Leader|SpriteTile/Leaders/homer</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="str">
-        <f>CONCATENATE(Civilopedia!A45,"|",Civilopedia!B45)</f>
-        <v>0-Julius Caesar|Leader</v>
+        <f>CONCATENATE(Civilopedia!A45,"|",Civilopedia!B45,"|",Civilopedia!E45)</f>
+        <v>0-Julius Caesar|Leader|SpriteTile/Leaders/julius_caesar</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="str">
-        <f>CONCATENATE(Civilopedia!A46,"|",Civilopedia!B46)</f>
-        <v>0-Moses|Leader</v>
+        <f>CONCATENATE(Civilopedia!A46,"|",Civilopedia!B46,"|",Civilopedia!E46)</f>
+        <v>0-Moses|Leader|SpriteTile/Leaders/moses</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="str">
-        <f>CONCATENATE(Civilopedia!A47,"|",Civilopedia!B47)</f>
-        <v>1-Christopher Columbus|Leader</v>
+        <f>CONCATENATE(Civilopedia!A47,"|",Civilopedia!B47,"|",Civilopedia!E47)</f>
+        <v>1-Christopher Columbus|Leader|SpriteTile/Leaders/christopher_columbus</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="str">
-        <f>CONCATENATE(Civilopedia!A48,"|",Civilopedia!B48)</f>
-        <v>1-Genghis Khan|Leader</v>
+        <f>CONCATENATE(Civilopedia!A48,"|",Civilopedia!B48,"|",Civilopedia!E48)</f>
+        <v>1-Genghis Khan|Leader|SpriteTile/Leaders/genghis_khan</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="str">
-        <f>CONCATENATE(Civilopedia!A49,"|",Civilopedia!B49)</f>
-        <v>1-Joan of Arc|Leader</v>
+        <f>CONCATENATE(Civilopedia!A49,"|",Civilopedia!B49,"|",Civilopedia!E49)</f>
+        <v>1-Joan of Arc|Leader|SpriteTile/Leaders/joan_of_arc</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="str">
-        <f>CONCATENATE(Civilopedia!A50,"|",Civilopedia!B50)</f>
-        <v>1-Leonardo Da Vinci|Leader</v>
+        <f>CONCATENATE(Civilopedia!A50,"|",Civilopedia!B50,"|",Civilopedia!E50)</f>
+        <v>1-Leonardo Da Vinci|Leader|SpriteTile/Leaders/leonardo_da_vinci</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="str">
-        <f>CONCATENATE(Civilopedia!A51,"|",Civilopedia!B51)</f>
-        <v>1-Michelangelo|Leader</v>
+        <f>CONCATENATE(Civilopedia!A51,"|",Civilopedia!B51,"|",Civilopedia!E51)</f>
+        <v>1-Michelangelo|Leader|SpriteTile/Leaders/michelangelo</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="str">
-        <f>CONCATENATE(Civilopedia!A52,"|",Civilopedia!B52)</f>
-        <v>2-Frederick Barbarossa|Leader</v>
+        <f>CONCATENATE(Civilopedia!A52,"|",Civilopedia!B52,"|",Civilopedia!E52)</f>
+        <v>2-Frederick Barbarossa|Leader|SpriteTile/Leaders/frederick_barbarossa</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="str">
-        <f>CONCATENATE(Civilopedia!A53,"|",Civilopedia!B53)</f>
-        <v>2-Isaac Newton|Leader</v>
+        <f>CONCATENATE(Civilopedia!A53,"|",Civilopedia!B53,"|",Civilopedia!E53)</f>
+        <v>2-Isaac Newton|Leader|SpriteTile/Leaders/isaac_newton</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="str">
-        <f>CONCATENATE(Civilopedia!A54,"|",Civilopedia!B54)</f>
-        <v>2-James Cook|Leader</v>
+        <f>CONCATENATE(Civilopedia!A54,"|",Civilopedia!B54,"|",Civilopedia!E54)</f>
+        <v>2-James Cook|Leader|SpriteTile/Leaders/james_cook</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="str">
-        <f>CONCATENATE(Civilopedia!A55,"|",Civilopedia!B55)</f>
-        <v>2-Maximillien Robespierre|Leader</v>
+        <f>CONCATENATE(Civilopedia!A55,"|",Civilopedia!B55,"|",Civilopedia!E55)</f>
+        <v>2-Maximillien Robespierre|Leader|SpriteTile/Leaders/maximillien_robespierre</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="str">
-        <f>CONCATENATE(Civilopedia!A56,"|",Civilopedia!B56)</f>
-        <v>2-Napoleon Bonaparte|Leader</v>
+        <f>CONCATENATE(Civilopedia!A56,"|",Civilopedia!B56,"|",Civilopedia!E56)</f>
+        <v>2-Napoleon Bonaparte|Leader|SpriteTile/Leaders/napoleon_bonaparte</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="str">
-        <f>CONCATENATE(Civilopedia!A57,"|",Civilopedia!B57)</f>
-        <v>2-William Shakespeare|Leader</v>
+        <f>CONCATENATE(Civilopedia!A57,"|",Civilopedia!B57,"|",Civilopedia!E57)</f>
+        <v>2-William Shakespeare|Leader|SpriteTile/Leaders/william_shakespeare</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="str">
-        <f>CONCATENATE(Civilopedia!A58,"|",Civilopedia!B58)</f>
-        <v>3-Albert Einstein|Leader</v>
+        <f>CONCATENATE(Civilopedia!A58,"|",Civilopedia!B58,"|",Civilopedia!E58)</f>
+        <v>3-Albert Einstein|Leader|SpriteTile/Leaders/albert_einstein</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="str">
-        <f>CONCATENATE(Civilopedia!A59,"|",Civilopedia!B59)</f>
-        <v>3-Bill Gates|Leader</v>
+        <f>CONCATENATE(Civilopedia!A59,"|",Civilopedia!B59,"|",Civilopedia!E59)</f>
+        <v>3-Bill Gates|Leader|SpriteTile/Leaders/bill_gates</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="str">
-        <f>CONCATENATE(Civilopedia!A60,"|",Civilopedia!B60)</f>
-        <v>3-Charles Chaplin|Leader</v>
+        <f>CONCATENATE(Civilopedia!A60,"|",Civilopedia!B60,"|",Civilopedia!E60)</f>
+        <v>3-Charles Chaplin|Leader|SpriteTile/Leaders/charles_chaplin</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="str">
-        <f>CONCATENATE(Civilopedia!A61,"|",Civilopedia!B61)</f>
-        <v>3-Mahatma Gandhi|Leader</v>
+        <f>CONCATENATE(Civilopedia!A61,"|",Civilopedia!B61,"|",Civilopedia!E61)</f>
+        <v>3-Mahatma Gandhi|Leader|SpriteTile/Leaders/mahatma_gandhi</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="str">
-        <f>CONCATENATE(Civilopedia!A62,"|",Civilopedia!B62)</f>
-        <v>3-Sid Meier|Leader</v>
+        <f>CONCATENATE(Civilopedia!A62,"|",Civilopedia!B62,"|",Civilopedia!E62)</f>
+        <v>3-Sid Meier|Leader|SpriteTile/Leaders/sid_meier</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="str">
-        <f>CONCATENATE(Civilopedia!A63,"|",Civilopedia!B63)</f>
-        <v>3-Winston Churchill|Leader</v>
+        <f>CONCATENATE(Civilopedia!A63,"|",Civilopedia!B63,"|",Civilopedia!E63)</f>
+        <v>3-Winston Churchill|Leader|SpriteTile/Leaders/winston_churchill</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="str">
-        <f>CONCATENATE(Civilopedia!A64,"|",Civilopedia!B64)</f>
-        <v>3-Air Forces|MilitaryTechAirForce</v>
+        <f>CONCATENATE(Civilopedia!A64,"|",Civilopedia!B64,"|",Civilopedia!E64)</f>
+        <v>3-Air Forces|MilitaryTechAirForce|SpriteTile/MilitaryTechAirForces/air_forces</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="str">
-        <f>CONCATENATE(Civilopedia!A65,"|",Civilopedia!B65)</f>
-        <v>2-Cannon|MilitaryTechArtillery</v>
+        <f>CONCATENATE(Civilopedia!A65,"|",Civilopedia!B65,"|",Civilopedia!E65)</f>
+        <v>2-Cannon|MilitaryTechArtillery|SpriteTile/MilitaryTechArtillerys/cannon</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="str">
-        <f>CONCATENATE(Civilopedia!A66,"|",Civilopedia!B66)</f>
-        <v>3-Rockets|MilitaryTechArtillery</v>
+        <f>CONCATENATE(Civilopedia!A66,"|",Civilopedia!B66,"|",Civilopedia!E66)</f>
+        <v>3-Rockets|MilitaryTechArtillery|SpriteTile/MilitaryTechArtillerys/rockets</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="str">
-        <f>CONCATENATE(Civilopedia!A67,"|",Civilopedia!B67)</f>
-        <v>1-Knights|MilitaryTechCavalry</v>
+        <f>CONCATENATE(Civilopedia!A67,"|",Civilopedia!B67,"|",Civilopedia!E67)</f>
+        <v>1-Knights|MilitaryTechCavalry|SpriteTile/MilitaryTechCavalrys/knights</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="str">
-        <f>CONCATENATE(Civilopedia!A68,"|",Civilopedia!B68)</f>
-        <v>2-Cavalrymen|MilitaryTechCavalry</v>
+        <f>CONCATENATE(Civilopedia!A68,"|",Civilopedia!B68,"|",Civilopedia!E68)</f>
+        <v>2-Cavalrymen|MilitaryTechCavalry|SpriteTile/MilitaryTechCavalrys/cavalrymen</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="str">
-        <f>CONCATENATE(Civilopedia!A69,"|",Civilopedia!B69)</f>
-        <v>3-Tanks|MilitaryTechCavalry</v>
+        <f>CONCATENATE(Civilopedia!A69,"|",Civilopedia!B69,"|",Civilopedia!E69)</f>
+        <v>3-Tanks|MilitaryTechCavalry|SpriteTile/MilitaryTechCavalrys/tanks</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="str">
-        <f>CONCATENATE(Civilopedia!A70,"|",Civilopedia!B70)</f>
-        <v>1-Swordsmen|MilitaryTechInfantry</v>
+        <f>CONCATENATE(Civilopedia!A70,"|",Civilopedia!B70,"|",Civilopedia!E70)</f>
+        <v>1-Swordsmen|MilitaryTechInfantry|SpriteTile/MilitaryTechInfantrys/swordsmen</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="str">
-        <f>CONCATENATE(Civilopedia!A71,"|",Civilopedia!B71)</f>
-        <v>2-Riflemen|MilitaryTechInfantry</v>
+        <f>CONCATENATE(Civilopedia!A71,"|",Civilopedia!B71,"|",Civilopedia!E71)</f>
+        <v>2-Riflemen|MilitaryTechInfantry|SpriteTile/MilitaryTechInfantrys/riflemen</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="str">
-        <f>CONCATENATE(Civilopedia!A72,"|",Civilopedia!B72)</f>
-        <v>3-Modern Infantry|MilitaryTechInfantry</v>
+        <f>CONCATENATE(Civilopedia!A72,"|",Civilopedia!B72,"|",Civilopedia!E72)</f>
+        <v>3-Modern Infantry|MilitaryTechInfantry|SpriteTile/MilitaryTechInfantrys/modern_infantry</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="str">
-        <f>CONCATENATE(Civilopedia!A73,"|",Civilopedia!B73)</f>
-        <v>1-Irrigation|ResourceTechFarm</v>
+        <f>CONCATENATE(Civilopedia!A73,"|",Civilopedia!B73,"|",Civilopedia!E73)</f>
+        <v>1-Irrigation|ResourceTechFarm|SpriteTile/ResourceTechFarms/irrigation</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="str">
-        <f>CONCATENATE(Civilopedia!A74,"|",Civilopedia!B74)</f>
-        <v>2-Selective Breeding|ResourceTechFarm</v>
+        <f>CONCATENATE(Civilopedia!A74,"|",Civilopedia!B74,"|",Civilopedia!E74)</f>
+        <v>2-Selective Breeding|ResourceTechFarm|SpriteTile/ResourceTechFarms/selective_breeding</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="str">
-        <f>CONCATENATE(Civilopedia!A75,"|",Civilopedia!B75)</f>
-        <v>3-Mechanized Agriculture|ResourceTechFarm</v>
+        <f>CONCATENATE(Civilopedia!A75,"|",Civilopedia!B75,"|",Civilopedia!E75)</f>
+        <v>3-Mechanized Agriculture|ResourceTechFarm|SpriteTile/ResourceTechFarms/mechanized_agriculture</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="str">
-        <f>CONCATENATE(Civilopedia!A76,"|",Civilopedia!B76)</f>
-        <v>1-Iron|ResourceTechMine</v>
+        <f>CONCATENATE(Civilopedia!A76,"|",Civilopedia!B76,"|",Civilopedia!E76)</f>
+        <v>1-Iron|ResourceTechMine|SpriteTile/ResourceTechMines/iron</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="str">
-        <f>CONCATENATE(Civilopedia!A77,"|",Civilopedia!B77)</f>
-        <v>2-Coal|ResourceTechMine</v>
+        <f>CONCATENATE(Civilopedia!A77,"|",Civilopedia!B77,"|",Civilopedia!E77)</f>
+        <v>2-Coal|ResourceTechMine|SpriteTile/ResourceTechMines/coal</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="str">
-        <f>CONCATENATE(Civilopedia!A78,"|",Civilopedia!B78)</f>
-        <v>3-Oil|ResourceTechMine</v>
+        <f>CONCATENATE(Civilopedia!A78,"|",Civilopedia!B78,"|",Civilopedia!E78)</f>
+        <v>3-Oil|ResourceTechMine|SpriteTile/ResourceTechMines/oil</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="str">
-        <f>CONCATENATE(Civilopedia!A79,"|",Civilopedia!B79)</f>
-        <v>1-Code of Laws|SpecialTechCivil</v>
+        <f>CONCATENATE(Civilopedia!A79,"|",Civilopedia!B79,"|",Civilopedia!E79)</f>
+        <v>1-Code of Laws|SpecialTechCivil|SpriteTile/SpecialTechCivils/code_of_laws</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="str">
-        <f>CONCATENATE(Civilopedia!A80,"|",Civilopedia!B80)</f>
-        <v>2-Justice System|SpecialTechCivil</v>
+        <f>CONCATENATE(Civilopedia!A80,"|",Civilopedia!B80,"|",Civilopedia!E80)</f>
+        <v>2-Justice System|SpecialTechCivil|SpriteTile/SpecialTechCivils/justice_system</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="str">
-        <f>CONCATENATE(Civilopedia!A81,"|",Civilopedia!B81)</f>
-        <v>3-Civil Service|SpecialTechCivil</v>
+        <f>CONCATENATE(Civilopedia!A81,"|",Civilopedia!B81,"|",Civilopedia!E81)</f>
+        <v>3-Civil Service|SpecialTechCivil|SpriteTile/SpecialTechCivils/civil_service</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="str">
-        <f>CONCATENATE(Civilopedia!A82,"|",Civilopedia!B82)</f>
-        <v>1-Masonry|SpecialTechEngineering</v>
+        <f>CONCATENATE(Civilopedia!A82,"|",Civilopedia!B82,"|",Civilopedia!E82)</f>
+        <v>1-Masonry|SpecialTechEngineering|SpriteTile/SpecialTechEngineerings/masonry</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="str">
-        <f>CONCATENATE(Civilopedia!A83,"|",Civilopedia!B83)</f>
-        <v>2-Architecture|SpecialTechEngineering</v>
+        <f>CONCATENATE(Civilopedia!A83,"|",Civilopedia!B83,"|",Civilopedia!E83)</f>
+        <v>2-Architecture|SpecialTechEngineering|SpriteTile/SpecialTechEngineerings/architecture</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="str">
-        <f>CONCATENATE(Civilopedia!A84,"|",Civilopedia!B84)</f>
-        <v>3-Engineering|SpecialTechEngineering</v>
+        <f>CONCATENATE(Civilopedia!A84,"|",Civilopedia!B84,"|",Civilopedia!E84)</f>
+        <v>3-Engineering|SpecialTechEngineering|SpriteTile/SpecialTechEngineerings/engineering</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="str">
-        <f>CONCATENATE(Civilopedia!A85,"|",Civilopedia!B85)</f>
-        <v>1-Cartography|SpecialTechExploration</v>
+        <f>CONCATENATE(Civilopedia!A85,"|",Civilopedia!B85,"|",Civilopedia!E85)</f>
+        <v>1-Cartography|SpecialTechExploration|SpriteTile/SpecialTechExplorations/cartography</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="str">
-        <f>CONCATENATE(Civilopedia!A86,"|",Civilopedia!B86)</f>
-        <v>2-Navigation|SpecialTechExploration</v>
+        <f>CONCATENATE(Civilopedia!A86,"|",Civilopedia!B86,"|",Civilopedia!E86)</f>
+        <v>2-Navigation|SpecialTechExploration|SpriteTile/SpecialTechExplorations/navigation</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="str">
-        <f>CONCATENATE(Civilopedia!A87,"|",Civilopedia!B87)</f>
-        <v>3-Satellites|SpecialTechExploration</v>
+        <f>CONCATENATE(Civilopedia!A87,"|",Civilopedia!B87,"|",Civilopedia!E87)</f>
+        <v>3-Satellites|SpecialTechExploration|SpriteTile/SpecialTechExplorations/satellites</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="str">
-        <f>CONCATENATE(Civilopedia!A88,"|",Civilopedia!B88)</f>
-        <v>1-Warfare|SpecialTechMilitary</v>
+        <f>CONCATENATE(Civilopedia!A88,"|",Civilopedia!B88,"|",Civilopedia!E88)</f>
+        <v>1-Warfare|SpecialTechMilitary|SpriteTile/SpecialTechMilitarys/warfare</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="str">
-        <f>CONCATENATE(Civilopedia!A89,"|",Civilopedia!B89)</f>
-        <v>2-Strategy|SpecialTechMilitary</v>
+        <f>CONCATENATE(Civilopedia!A89,"|",Civilopedia!B89,"|",Civilopedia!E89)</f>
+        <v>2-Strategy|SpecialTechMilitary|SpriteTile/SpecialTechMilitarys/strategy</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="str">
-        <f>CONCATENATE(Civilopedia!A90,"|",Civilopedia!B90)</f>
-        <v>3-Military Theory|SpecialTechMilitary</v>
+        <f>CONCATENATE(Civilopedia!A90,"|",Civilopedia!B90,"|",Civilopedia!E90)</f>
+        <v>3-Military Theory|SpecialTechMilitary|SpriteTile/SpecialTechMilitarys/military_theory</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="str">
-        <f>CONCATENATE(Civilopedia!A91,"|",Civilopedia!B91)</f>
-        <v>1-Bread &amp; Circuses|UrbanTechArena</v>
+        <f>CONCATENATE(Civilopedia!A91,"|",Civilopedia!B91,"|",Civilopedia!E91)</f>
+        <v>1-Bread &amp; Circuses|UrbanTechArena|SpriteTile/UrbanTechArenas/bread_&amp;_circuses</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="str">
-        <f>CONCATENATE(Civilopedia!A92,"|",Civilopedia!B92)</f>
-        <v>2-Team Sports|UrbanTechArena</v>
+        <f>CONCATENATE(Civilopedia!A92,"|",Civilopedia!B92,"|",Civilopedia!E92)</f>
+        <v>2-Team Sports|UrbanTechArena|SpriteTile/UrbanTechArenas/team_sports</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="str">
-        <f>CONCATENATE(Civilopedia!A93,"|",Civilopedia!B93)</f>
-        <v>3-Professional Sports|UrbanTechArena</v>
+        <f>CONCATENATE(Civilopedia!A93,"|",Civilopedia!B93,"|",Civilopedia!E93)</f>
+        <v>3-Professional Sports|UrbanTechArena|SpriteTile/UrbanTechArenas/professional_sports</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="str">
-        <f>CONCATENATE(Civilopedia!A94,"|",Civilopedia!B94)</f>
-        <v>1-Alchemy|UrbanTechLab</v>
+        <f>CONCATENATE(Civilopedia!A94,"|",Civilopedia!B94,"|",Civilopedia!E94)</f>
+        <v>1-Alchemy|UrbanTechLab|SpriteTile/UrbanTechLabs/alchemy</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="str">
-        <f>CONCATENATE(Civilopedia!A95,"|",Civilopedia!B95)</f>
-        <v>2-Scientific Method|UrbanTechLab</v>
+        <f>CONCATENATE(Civilopedia!A95,"|",Civilopedia!B95,"|",Civilopedia!E95)</f>
+        <v>2-Scientific Method|UrbanTechLab|SpriteTile/UrbanTechLabs/scientific_method</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="str">
-        <f>CONCATENATE(Civilopedia!A96,"|",Civilopedia!B96)</f>
-        <v>3-Computers|UrbanTechLab</v>
+        <f>CONCATENATE(Civilopedia!A96,"|",Civilopedia!B96,"|",Civilopedia!E96)</f>
+        <v>3-Computers|UrbanTechLab|SpriteTile/UrbanTechLabs/computers</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="str">
-        <f>CONCATENATE(Civilopedia!A97,"|",Civilopedia!B97)</f>
-        <v>1-Printing Press|UrbanTechLibrary</v>
+        <f>CONCATENATE(Civilopedia!A97,"|",Civilopedia!B97,"|",Civilopedia!E97)</f>
+        <v>1-Printing Press|UrbanTechLibrary|SpriteTile/UrbanTechLibrarys/printing_press</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="str">
-        <f>CONCATENATE(Civilopedia!A98,"|",Civilopedia!B98)</f>
-        <v>2-Journalism|UrbanTechLibrary</v>
+        <f>CONCATENATE(Civilopedia!A98,"|",Civilopedia!B98,"|",Civilopedia!E98)</f>
+        <v>2-Journalism|UrbanTechLibrary|SpriteTile/UrbanTechLibrarys/journalism</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="str">
-        <f>CONCATENATE(Civilopedia!A99,"|",Civilopedia!B99)</f>
-        <v>3-Multimedia|UrbanTechLibrary</v>
+        <f>CONCATENATE(Civilopedia!A99,"|",Civilopedia!B99,"|",Civilopedia!E99)</f>
+        <v>3-Multimedia|UrbanTechLibrary|SpriteTile/UrbanTechLibrarys/multimedia</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="str">
-        <f>CONCATENATE(Civilopedia!A100,"|",Civilopedia!B100)</f>
-        <v>1-Theology|UrbanTechTemple</v>
+        <f>CONCATENATE(Civilopedia!A100,"|",Civilopedia!B100,"|",Civilopedia!E100)</f>
+        <v>1-Theology|UrbanTechTemple|SpriteTile/UrbanTechTemples/theology</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="str">
-        <f>CONCATENATE(Civilopedia!A101,"|",Civilopedia!B101)</f>
-        <v>2-Organized Religion|UrbanTechTemple</v>
+        <f>CONCATENATE(Civilopedia!A101,"|",Civilopedia!B101,"|",Civilopedia!E101)</f>
+        <v>2-Organized Religion|UrbanTechTemple|SpriteTile/UrbanTechTemples/organized_religion</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="str">
-        <f>CONCATENATE(Civilopedia!A102,"|",Civilopedia!B102)</f>
-        <v>1-Drama|UrbanTechTheater</v>
+        <f>CONCATENATE(Civilopedia!A102,"|",Civilopedia!B102,"|",Civilopedia!E102)</f>
+        <v>1-Drama|UrbanTechTheater|SpriteTile/UrbanTechTheaters/drama</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="str">
-        <f>CONCATENATE(Civilopedia!A103,"|",Civilopedia!B103)</f>
-        <v>2-Opera|UrbanTechTheater</v>
+        <f>CONCATENATE(Civilopedia!A103,"|",Civilopedia!B103,"|",Civilopedia!E103)</f>
+        <v>2-Opera|UrbanTechTheater|SpriteTile/UrbanTechTheaters/opera</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="str">
-        <f>CONCATENATE(Civilopedia!A104,"|",Civilopedia!B104)</f>
-        <v>3-Movies|UrbanTechTheater</v>
+        <f>CONCATENATE(Civilopedia!A104,"|",Civilopedia!B104,"|",Civilopedia!E104)</f>
+        <v>3-Movies|UrbanTechTheater|SpriteTile/UrbanTechTheaters/movies</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="str">
-        <f>CONCATENATE(Civilopedia!A105,"|",Civilopedia!B105)</f>
-        <v>0-Colossus|Wonder</v>
+        <f>CONCATENATE(Civilopedia!A105,"|",Civilopedia!B105,"|",Civilopedia!E105)</f>
+        <v>0-Colossus|Wonder|SpriteTile/Wonders/colossus</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="str">
-        <f>CONCATENATE(Civilopedia!A106,"|",Civilopedia!B106)</f>
-        <v>0-Hanging Gardens|Wonder</v>
+        <f>CONCATENATE(Civilopedia!A106,"|",Civilopedia!B106,"|",Civilopedia!E106)</f>
+        <v>0-Hanging Gardens|Wonder|SpriteTile/Wonders/hanging_gardens</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="str">
-        <f>CONCATENATE(Civilopedia!A107,"|",Civilopedia!B107)</f>
-        <v>0-Library of Alexandria|Wonder</v>
+        <f>CONCATENATE(Civilopedia!A107,"|",Civilopedia!B107,"|",Civilopedia!E107)</f>
+        <v>0-Library of Alexandria|Wonder|SpriteTile/Wonders/library_of_alexandria</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="str">
-        <f>CONCATENATE(Civilopedia!A108,"|",Civilopedia!B108)</f>
-        <v>0-Pyramids|Wonder</v>
+        <f>CONCATENATE(Civilopedia!A108,"|",Civilopedia!B108,"|",Civilopedia!E108)</f>
+        <v>0-Pyramids|Wonder|SpriteTile/Wonders/pyramids</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="str">
-        <f>CONCATENATE(Civilopedia!A109,"|",Civilopedia!B109)</f>
-        <v>1-Great Wall|Wonder</v>
+        <f>CONCATENATE(Civilopedia!A109,"|",Civilopedia!B109,"|",Civilopedia!E109)</f>
+        <v>1-Great Wall|Wonder|SpriteTile/Wonders/great_wall</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="str">
-        <f>CONCATENATE(Civilopedia!A110,"|",Civilopedia!B110)</f>
-        <v>1-St. Peter's Basilica|Wonder</v>
+        <f>CONCATENATE(Civilopedia!A110,"|",Civilopedia!B110,"|",Civilopedia!E110)</f>
+        <v>1-St. Peter's Basilica|Wonder|SpriteTile/Wonders/st._peter's_basilica</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="str">
-        <f>CONCATENATE(Civilopedia!A111,"|",Civilopedia!B111)</f>
-        <v>1-Taj Mahal|Wonder</v>
+        <f>CONCATENATE(Civilopedia!A111,"|",Civilopedia!B111,"|",Civilopedia!E111)</f>
+        <v>1-Taj Mahal|Wonder|SpriteTile/Wonders/taj_mahal</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="str">
-        <f>CONCATENATE(Civilopedia!A112,"|",Civilopedia!B112)</f>
-        <v>1-Universitas Carolina|Wonder</v>
+        <f>CONCATENATE(Civilopedia!A112,"|",Civilopedia!B112,"|",Civilopedia!E112)</f>
+        <v>1-Universitas Carolina|Wonder|SpriteTile/Wonders/universitas_carolina</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="str">
-        <f>CONCATENATE(Civilopedia!A113,"|",Civilopedia!B113)</f>
-        <v>2-Eiffel Tower|Wonder</v>
+        <f>CONCATENATE(Civilopedia!A113,"|",Civilopedia!B113,"|",Civilopedia!E113)</f>
+        <v>2-Eiffel Tower|Wonder|SpriteTile/Wonders/eiffel_tower</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="str">
-        <f>CONCATENATE(Civilopedia!A114,"|",Civilopedia!B114)</f>
-        <v>2-Kremlin|Wonder</v>
+        <f>CONCATENATE(Civilopedia!A114,"|",Civilopedia!B114,"|",Civilopedia!E114)</f>
+        <v>2-Kremlin|Wonder|SpriteTile/Wonders/kremlin</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="str">
-        <f>CONCATENATE(Civilopedia!A115,"|",Civilopedia!B115)</f>
-        <v>2-Ocean Liner|Wonder</v>
+        <f>CONCATENATE(Civilopedia!A115,"|",Civilopedia!B115,"|",Civilopedia!E115)</f>
+        <v>2-Ocean Liner|Wonder|SpriteTile/Wonders/ocean_liner</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="str">
-        <f>CONCATENATE(Civilopedia!A116,"|",Civilopedia!B116)</f>
-        <v>2-Transcontinental Railroad|Wonder</v>
+        <f>CONCATENATE(Civilopedia!A116,"|",Civilopedia!B116,"|",Civilopedia!E116)</f>
+        <v>2-Transcontinental Railroad|Wonder|SpriteTile/Wonders/transcontinental_railroad</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="str">
-        <f>CONCATENATE(Civilopedia!A117,"|",Civilopedia!B117)</f>
-        <v>3-Fast Food Chains|Wonder</v>
+        <f>CONCATENATE(Civilopedia!A117,"|",Civilopedia!B117,"|",Civilopedia!E117)</f>
+        <v>3-Fast Food Chains|Wonder|SpriteTile/Wonders/fast_food_chains</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="str">
-        <f>CONCATENATE(Civilopedia!A118,"|",Civilopedia!B118)</f>
-        <v>3-First Space Flight|Wonder</v>
+        <f>CONCATENATE(Civilopedia!A118,"|",Civilopedia!B118,"|",Civilopedia!E118)</f>
+        <v>3-First Space Flight|Wonder|SpriteTile/Wonders/first_space_flight</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="str">
-        <f>CONCATENATE(Civilopedia!A119,"|",Civilopedia!B119)</f>
-        <v>3-Hollywood|Wonder</v>
+        <f>CONCATENATE(Civilopedia!A119,"|",Civilopedia!B119,"|",Civilopedia!E119)</f>
+        <v>3-Hollywood|Wonder|SpriteTile/Wonders/hollywood</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="str">
-        <f>CONCATENATE(Civilopedia!A120,"|",Civilopedia!B120)</f>
-        <v>3-Internet|Wonder</v>
+        <f>CONCATENATE(Civilopedia!A120,"|",Civilopedia!B120,"|",Civilopedia!E120)</f>
+        <v>3-Internet|Wonder|SpriteTile/Wonders/internet</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
@@ -3446,6 +4438,10 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Add a pc version
</commit_message>
<xml_diff>
--- a/Reference/Civilopedia.xlsx
+++ b/Reference/Civilopedia.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16729"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Civilopedia" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="146">
   <si>
     <t>Internal Id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -461,7 +461,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Image Name</t>
+    <t>Normal Image Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Small Image Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Normal Image Asset Path</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Special Image Asset Path</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Special Image Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -535,26 +551,30 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A1:F120" totalsRowShown="0">
-  <autoFilter ref="A1:F120"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A1:J120" totalsRowShown="0">
+  <autoFilter ref="A1:J120"/>
   <sortState ref="A2:D120">
     <sortCondition ref="B2:B120"/>
     <sortCondition ref="D2:D120"/>
     <sortCondition ref="C2:C120"/>
   </sortState>
-  <tableColumns count="6">
+  <tableColumns count="10">
     <tableColumn id="1" name="Internal Id" dataDxfId="2">
       <calculatedColumnFormula>CONCATENATE(D2,"-",C2)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" name="Card Type"/>
     <tableColumn id="3" name="Card Name"/>
     <tableColumn id="4" name="Age"/>
-    <tableColumn id="5" name="Small Image Asset Path" dataDxfId="0">
+    <tableColumn id="5" name="Small Image Asset Path" dataDxfId="1">
       <calculatedColumnFormula>_xlfn.CONCAT("SpriteTile/",B2,"s/",LOWER(SUBSTITUTE(C2," ","_")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Image Name" dataDxfId="1">
+    <tableColumn id="6" name="Small Image Name" dataDxfId="0">
       <calculatedColumnFormula>_xlfn.CONCAT(LOWER(SUBSTITUTE(C2," ","_")))</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="9" name="Normal Image Asset Path"/>
+    <tableColumn id="7" name="Normal Image Name"/>
+    <tableColumn id="10" name="Special Image Asset Path"/>
+    <tableColumn id="11" name="Special Image Name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -879,10 +899,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F120"/>
+  <dimension ref="A1:J120"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -892,9 +912,13 @@
     <col min="3" max="3" width="22.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="44.75" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.75" customWidth="1"/>
+    <col min="8" max="8" width="22.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -911,10 +935,22 @@
         <v>140</v>
       </c>
       <c r="F1" t="s">
+        <v>142</v>
+      </c>
+      <c r="G1" t="s">
+        <v>143</v>
+      </c>
+      <c r="H1" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I1" t="s">
+        <v>144</v>
+      </c>
+      <c r="J1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f t="shared" ref="A2:A33" si="0">CONCATENATE(D2,"-",C2)</f>
         <v>0-Cultural Heritage</v>
@@ -937,7 +973,7 @@
         <v>cultural_heritage</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f t="shared" si="0"/>
         <v>0-Engineering Genius</v>
@@ -960,7 +996,7 @@
         <v>engineering_genius</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>0-Frugality</v>
@@ -983,7 +1019,7 @@
         <v>frugality</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>0-Patriotism</v>
@@ -1006,7 +1042,7 @@
         <v>patriotism</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
         <v>0-Rich Land</v>
@@ -1029,7 +1065,7 @@
         <v>rich_land</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
         <v>0-Stockpile</v>
@@ -1052,7 +1088,7 @@
         <v>stockpile</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="str">
         <f t="shared" si="0"/>
         <v>0-Urban Growth</v>
@@ -1075,7 +1111,7 @@
         <v>urban_growth</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
         <v>1-Breakthrough</v>
@@ -1098,7 +1134,7 @@
         <v>breakthrough</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
         <v>1-Cultural Heritage</v>
@@ -1121,7 +1157,7 @@
         <v>cultural_heritage</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
         <v>1-Engineering Genius</v>
@@ -1144,7 +1180,7 @@
         <v>engineering_genius</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
         <v>1-Frugality</v>
@@ -1167,7 +1203,7 @@
         <v>frugality</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
         <v>1-Patriotism</v>
@@ -1190,7 +1226,7 @@
         <v>patriotism</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="str">
         <f t="shared" si="0"/>
         <v>1-Reserves</v>
@@ -1213,7 +1249,7 @@
         <v>reserves</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="str">
         <f t="shared" si="0"/>
         <v>1-Rich Land</v>
@@ -1236,7 +1272,7 @@
         <v>rich_land</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
         <v>1-Urban Growth</v>
@@ -3677,8 +3713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A120"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="T138" sqref="T138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>